<commit_message>
versao dia 06 Apresentacao
</commit_message>
<xml_diff>
--- a/Informacoes_Sistema/Cópia de Cópia de PLANILHA DE CUSTO ST E CUSTOS ALLES FEV-15 (6).xlsx
+++ b/Informacoes_Sistema/Cópia de Cópia de PLANILHA DE CUSTO ST E CUSTOS ALLES FEV-15 (6).xlsx
@@ -1,13 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <bookViews>
+    <workbookView xWindow="390" yWindow="555" windowWidth="19815" windowHeight="7365" activeTab="1"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Calculo de ST " sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Calculo de Venda " sheetId="2" r:id="rId5"/>
+    <sheet name="Calculo de ST " sheetId="1" r:id="rId1"/>
+    <sheet name="Calculo de Venda " sheetId="2" r:id="rId2"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -158,7 +161,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@"/>
     <numFmt numFmtId="165" formatCode="_-[$R$-416]\ * #,##0.00_-;\-[$R$-416]\ * #,##0.00_-;_-[$R$-416]\ * &quot;-&quot;??_-;_-@"/>
@@ -166,28 +169,31 @@
   </numFmts>
   <fonts count="6">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="14.0"/>
+      <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
     </font>
-    <font/>
     <font>
-      <sz val="14.0"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <color rgb="FFFFFFFF"/>
       <name val="Cambria"/>
     </font>
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
     </font>
     <font>
-      <sz val="12.0"/>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Cambria"/>
     </font>
@@ -197,7 +203,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -213,98 +219,108 @@
     </fill>
   </fills>
   <borders count="5">
-    <border/>
     <border>
       <left/>
-      <top/>
-      <bottom/>
-    </border>
-    <border>
-      <top/>
-      <bottom/>
-    </border>
-    <border>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="27">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="1" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="4" fillId="2" fontId="1" numFmtId="165" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf borderId="4" fillId="2" fontId="1" numFmtId="9" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="165" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="9" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="4" fillId="2" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="2" fontId="1" numFmtId="164" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="4" fillId="3" fontId="3" numFmtId="164" xfId="0" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="4" fillId="3" fontId="3" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="2" fontId="1" numFmtId="10" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="4" fillId="3" fontId="3" numFmtId="9" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="166" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="2" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="2" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="164" xfId="0" applyFont="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/worksheetdrawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/worksheetdrawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Escritório">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -462,7 +478,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln cap="flat" cmpd="sng" w="9525" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -471,13 +487,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln cap="flat" cmpd="sng" w="25400" algn="ctr">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln cap="flat" cmpd="sng" w="38100" algn="ctr">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -487,7 +503,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" rotWithShape="0" dir="5400000" dist="20000">
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -496,7 +512,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" rotWithShape="0" dir="5400000" dist="23000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -505,7 +521,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" rotWithShape="0" dir="5400000" dist="23000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -515,12 +531,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
+            <a:lightRig rig="threePt" dir="t">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT h="25400" w="63500"/>
+            <a:bevelT w="63500" h="25400"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -551,7 +567,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -570,7 +586,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -582,23 +598,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K100"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="23.86"/>
-    <col customWidth="1" min="2" max="2" width="15.86"/>
-    <col customWidth="1" min="3" max="3" width="9.29"/>
-    <col customWidth="1" min="4" max="4" width="15.14"/>
-    <col customWidth="1" min="5" max="11" width="9.14"/>
+    <col min="1" max="1" width="23.85546875" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" customWidth="1"/>
+    <col min="5" max="11" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18.0" customHeight="1">
+    <row r="1" spans="1:11" ht="18" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -613,14 +629,14 @@
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" ht="18.0" customHeight="1">
-      <c r="A2" s="2" t="s">
+    <row r="2" spans="1:11" ht="18" customHeight="1">
+      <c r="A2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="4"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="26"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
@@ -628,12 +644,12 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" ht="18.0" customHeight="1">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
+    <row r="3" spans="1:11" ht="18" customHeight="1">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
@@ -641,16 +657,16 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" ht="18.0" customHeight="1">
+    <row r="4" spans="1:11" ht="18" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
-      <c r="D4" s="6">
+      <c r="D4" s="3">
         <v>0.94</v>
       </c>
-      <c r="E4" s="7"/>
+      <c r="E4" s="4"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
@@ -658,19 +674,19 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" ht="18.0" customHeight="1">
+    <row r="5" spans="1:11" ht="18" customHeight="1">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="1"/>
-      <c r="C5" s="8">
+      <c r="C5" s="5">
         <v>0.1</v>
       </c>
-      <c r="D5" s="9" t="str">
+      <c r="D5" s="6">
         <f>D4*C5</f>
-        <v> R$  0.09 </v>
-      </c>
-      <c r="E5" s="7"/>
+        <v>9.4E-2</v>
+      </c>
+      <c r="E5" s="4"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -678,13 +694,13 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" ht="18.0" customHeight="1">
+    <row r="6" spans="1:11" ht="18" customHeight="1">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-      <c r="D6" s="9" t="str">
+      <c r="D6" s="6">
         <f>SUM(D4:D5)</f>
-        <v> R$  1.03 </v>
+        <v>1.034</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -694,17 +710,17 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" ht="18.0" customHeight="1">
+    <row r="7" spans="1:11" ht="18" customHeight="1">
       <c r="A7" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="1"/>
-      <c r="C7" s="8">
+      <c r="C7" s="5">
         <v>0.8</v>
       </c>
-      <c r="D7" s="9" t="str">
+      <c r="D7" s="6">
         <f>D4*C7</f>
-        <v> R$  0.75 </v>
+        <v>0.752</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -714,13 +730,13 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" ht="18.0" customHeight="1">
+    <row r="8" spans="1:11" ht="18" customHeight="1">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
-      <c r="D8" s="9" t="str">
+      <c r="D8" s="6">
         <f>D4+D5+D7</f>
-        <v> R$  1.79 </v>
+        <v>1.786</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -730,11 +746,11 @@
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" ht="18.0" customHeight="1">
+    <row r="9" spans="1:11" ht="18" customHeight="1">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
-      <c r="D9" s="9"/>
+      <c r="D9" s="6"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -743,17 +759,17 @@
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" ht="18.0" customHeight="1">
+    <row r="10" spans="1:11" ht="18" customHeight="1">
       <c r="A10" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="1"/>
-      <c r="C10" s="10">
+      <c r="C10" s="7">
         <v>0.18</v>
       </c>
-      <c r="D10" s="9" t="str">
+      <c r="D10" s="6">
         <f>D8*C10</f>
-        <v> R$  0.32 </v>
+        <v>0.32147999999999999</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
@@ -763,17 +779,17 @@
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" ht="18.0" customHeight="1">
+    <row r="11" spans="1:11" ht="18" customHeight="1">
       <c r="A11" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="1"/>
-      <c r="C11" s="8">
+      <c r="C11" s="5">
         <v>0.04</v>
       </c>
-      <c r="D11" s="9" t="str">
+      <c r="D11" s="6">
         <f>D4*C11</f>
-        <v> R$  0.04 </v>
+        <v>3.7600000000000001E-2</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
@@ -783,15 +799,15 @@
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" ht="18.0" customHeight="1">
+    <row r="12" spans="1:11" ht="18" customHeight="1">
       <c r="A12" s="1" t="s">
         <v>7</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
-      <c r="D12" s="9" t="str">
+      <c r="D12" s="6">
         <f>D10-D11</f>
-        <v> R$  0.28 </v>
+        <v>0.28387999999999997</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
@@ -801,11 +817,11 @@
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" ht="18.0" customHeight="1">
+    <row r="13" spans="1:11" ht="18" customHeight="1">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
-      <c r="D13" s="9"/>
+      <c r="D13" s="6"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
@@ -814,15 +830,15 @@
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" ht="18.0" customHeight="1">
+    <row r="14" spans="1:11" ht="18" customHeight="1">
       <c r="A14" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
-      <c r="D14" s="9" t="str">
+      <c r="D14" s="6">
         <f>D4+D5+D12</f>
-        <v> R$  1.32 </v>
+        <v>1.3178799999999999</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
@@ -832,11 +848,11 @@
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
     </row>
-    <row r="15" ht="18.0" customHeight="1">
+    <row r="15" spans="1:11" ht="18" customHeight="1">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
-      <c r="D15" s="9"/>
+      <c r="D15" s="6"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
@@ -845,7 +861,7 @@
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" ht="18.0" customHeight="1">
+    <row r="16" spans="1:11" ht="18" customHeight="1">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -858,7 +874,7 @@
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
     </row>
-    <row r="17" ht="18.0" customHeight="1">
+    <row r="17" spans="1:11" ht="18" customHeight="1">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -871,7 +887,7 @@
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
     </row>
-    <row r="18" ht="18.0" customHeight="1">
+    <row r="18" spans="1:11" ht="18" customHeight="1">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -884,7 +900,7 @@
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
     </row>
-    <row r="19" ht="18.0" customHeight="1">
+    <row r="19" spans="1:11" ht="18" customHeight="1">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -897,7 +913,7 @@
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" ht="18.0" customHeight="1">
+    <row r="20" spans="1:11" ht="18" customHeight="1">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -910,7 +926,7 @@
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
     </row>
-    <row r="21" ht="18.0" customHeight="1">
+    <row r="21" spans="1:11" ht="18" customHeight="1">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -923,7 +939,7 @@
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
     </row>
-    <row r="22" ht="18.0" customHeight="1">
+    <row r="22" spans="1:11" ht="18" customHeight="1">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -936,7 +952,7 @@
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
     </row>
-    <row r="23" ht="18.0" customHeight="1">
+    <row r="23" spans="1:11" ht="18" customHeight="1">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -949,7 +965,7 @@
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
     </row>
-    <row r="24" ht="18.0" customHeight="1">
+    <row r="24" spans="1:11" ht="18" customHeight="1">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -962,7 +978,7 @@
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
     </row>
-    <row r="25" ht="18.0" customHeight="1">
+    <row r="25" spans="1:11" ht="18" customHeight="1">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -975,7 +991,7 @@
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
     </row>
-    <row r="26" ht="18.0" customHeight="1">
+    <row r="26" spans="1:11" ht="18" customHeight="1">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -988,7 +1004,7 @@
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
     </row>
-    <row r="27" ht="18.0" customHeight="1">
+    <row r="27" spans="1:11" ht="18" customHeight="1">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1001,7 +1017,7 @@
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
     </row>
-    <row r="28" ht="18.0" customHeight="1">
+    <row r="28" spans="1:11" ht="18" customHeight="1">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1014,7 +1030,7 @@
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
     </row>
-    <row r="29" ht="18.0" customHeight="1">
+    <row r="29" spans="1:11" ht="18" customHeight="1">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -1027,7 +1043,7 @@
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
     </row>
-    <row r="30" ht="18.0" customHeight="1">
+    <row r="30" spans="1:11" ht="18" customHeight="1">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1040,7 +1056,7 @@
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
     </row>
-    <row r="31" ht="18.0" customHeight="1">
+    <row r="31" spans="1:11" ht="18" customHeight="1">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -1053,7 +1069,7 @@
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
     </row>
-    <row r="32" ht="18.0" customHeight="1">
+    <row r="32" spans="1:11" ht="18" customHeight="1">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -1066,7 +1082,7 @@
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
     </row>
-    <row r="33" ht="18.0" customHeight="1">
+    <row r="33" spans="1:11" ht="18" customHeight="1">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -1079,7 +1095,7 @@
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
     </row>
-    <row r="34" ht="18.0" customHeight="1">
+    <row r="34" spans="1:11" ht="18" customHeight="1">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1092,7 +1108,7 @@
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
     </row>
-    <row r="35" ht="18.0" customHeight="1">
+    <row r="35" spans="1:11" ht="18" customHeight="1">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -1105,7 +1121,7 @@
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
     </row>
-    <row r="36" ht="18.0" customHeight="1">
+    <row r="36" spans="1:11" ht="18" customHeight="1">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -1118,7 +1134,7 @@
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
     </row>
-    <row r="37" ht="18.0" customHeight="1">
+    <row r="37" spans="1:11" ht="18" customHeight="1">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -1131,7 +1147,7 @@
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
     </row>
-    <row r="38" ht="18.0" customHeight="1">
+    <row r="38" spans="1:11" ht="18" customHeight="1">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -1144,7 +1160,7 @@
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
     </row>
-    <row r="39" ht="18.0" customHeight="1">
+    <row r="39" spans="1:11" ht="18" customHeight="1">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -1157,7 +1173,7 @@
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
     </row>
-    <row r="40" ht="18.0" customHeight="1">
+    <row r="40" spans="1:11" ht="18" customHeight="1">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -1170,7 +1186,7 @@
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
     </row>
-    <row r="41" ht="18.0" customHeight="1">
+    <row r="41" spans="1:11" ht="18" customHeight="1">
       <c r="A41" s="1"/>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -1183,7 +1199,7 @@
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
     </row>
-    <row r="42" ht="18.0" customHeight="1">
+    <row r="42" spans="1:11" ht="18" customHeight="1">
       <c r="A42" s="1"/>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -1196,7 +1212,7 @@
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
     </row>
-    <row r="43" ht="18.0" customHeight="1">
+    <row r="43" spans="1:11" ht="18" customHeight="1">
       <c r="A43" s="1"/>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -1209,7 +1225,7 @@
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
     </row>
-    <row r="44" ht="18.0" customHeight="1">
+    <row r="44" spans="1:11" ht="18" customHeight="1">
       <c r="A44" s="1"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -1222,7 +1238,7 @@
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
     </row>
-    <row r="45" ht="18.0" customHeight="1">
+    <row r="45" spans="1:11" ht="18" customHeight="1">
       <c r="A45" s="1"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -1235,7 +1251,7 @@
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
     </row>
-    <row r="46" ht="18.0" customHeight="1">
+    <row r="46" spans="1:11" ht="18" customHeight="1">
       <c r="A46" s="1"/>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -1248,7 +1264,7 @@
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
     </row>
-    <row r="47" ht="18.0" customHeight="1">
+    <row r="47" spans="1:11" ht="18" customHeight="1">
       <c r="A47" s="1"/>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -1261,7 +1277,7 @@
       <c r="J47" s="1"/>
       <c r="K47" s="1"/>
     </row>
-    <row r="48" ht="18.0" customHeight="1">
+    <row r="48" spans="1:11" ht="18" customHeight="1">
       <c r="A48" s="1"/>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -1274,7 +1290,7 @@
       <c r="J48" s="1"/>
       <c r="K48" s="1"/>
     </row>
-    <row r="49" ht="18.0" customHeight="1">
+    <row r="49" spans="1:11" ht="18" customHeight="1">
       <c r="A49" s="1"/>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -1287,7 +1303,7 @@
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
     </row>
-    <row r="50" ht="18.0" customHeight="1">
+    <row r="50" spans="1:11" ht="18" customHeight="1">
       <c r="A50" s="1"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -1300,7 +1316,7 @@
       <c r="J50" s="1"/>
       <c r="K50" s="1"/>
     </row>
-    <row r="51" ht="18.0" customHeight="1">
+    <row r="51" spans="1:11" ht="18" customHeight="1">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -1313,7 +1329,7 @@
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
     </row>
-    <row r="52" ht="18.0" customHeight="1">
+    <row r="52" spans="1:11" ht="18" customHeight="1">
       <c r="A52" s="1"/>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -1326,7 +1342,7 @@
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
     </row>
-    <row r="53" ht="18.0" customHeight="1">
+    <row r="53" spans="1:11" ht="18" customHeight="1">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -1339,7 +1355,7 @@
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
     </row>
-    <row r="54" ht="18.0" customHeight="1">
+    <row r="54" spans="1:11" ht="18" customHeight="1">
       <c r="A54" s="1"/>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -1352,7 +1368,7 @@
       <c r="J54" s="1"/>
       <c r="K54" s="1"/>
     </row>
-    <row r="55" ht="18.0" customHeight="1">
+    <row r="55" spans="1:11" ht="18" customHeight="1">
       <c r="A55" s="1"/>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -1365,7 +1381,7 @@
       <c r="J55" s="1"/>
       <c r="K55" s="1"/>
     </row>
-    <row r="56" ht="18.0" customHeight="1">
+    <row r="56" spans="1:11" ht="18" customHeight="1">
       <c r="A56" s="1"/>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -1378,7 +1394,7 @@
       <c r="J56" s="1"/>
       <c r="K56" s="1"/>
     </row>
-    <row r="57" ht="18.0" customHeight="1">
+    <row r="57" spans="1:11" ht="18" customHeight="1">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -1391,7 +1407,7 @@
       <c r="J57" s="1"/>
       <c r="K57" s="1"/>
     </row>
-    <row r="58" ht="18.0" customHeight="1">
+    <row r="58" spans="1:11" ht="18" customHeight="1">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -1404,7 +1420,7 @@
       <c r="J58" s="1"/>
       <c r="K58" s="1"/>
     </row>
-    <row r="59" ht="18.0" customHeight="1">
+    <row r="59" spans="1:11" ht="18" customHeight="1">
       <c r="A59" s="1"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -1417,7 +1433,7 @@
       <c r="J59" s="1"/>
       <c r="K59" s="1"/>
     </row>
-    <row r="60" ht="18.0" customHeight="1">
+    <row r="60" spans="1:11" ht="18" customHeight="1">
       <c r="A60" s="1"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -1430,7 +1446,7 @@
       <c r="J60" s="1"/>
       <c r="K60" s="1"/>
     </row>
-    <row r="61" ht="18.0" customHeight="1">
+    <row r="61" spans="1:11" ht="18" customHeight="1">
       <c r="A61" s="1"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -1443,7 +1459,7 @@
       <c r="J61" s="1"/>
       <c r="K61" s="1"/>
     </row>
-    <row r="62" ht="18.0" customHeight="1">
+    <row r="62" spans="1:11" ht="18" customHeight="1">
       <c r="A62" s="1"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -1456,7 +1472,7 @@
       <c r="J62" s="1"/>
       <c r="K62" s="1"/>
     </row>
-    <row r="63" ht="18.0" customHeight="1">
+    <row r="63" spans="1:11" ht="18" customHeight="1">
       <c r="A63" s="1"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -1469,7 +1485,7 @@
       <c r="J63" s="1"/>
       <c r="K63" s="1"/>
     </row>
-    <row r="64" ht="18.0" customHeight="1">
+    <row r="64" spans="1:11" ht="18" customHeight="1">
       <c r="A64" s="1"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -1482,7 +1498,7 @@
       <c r="J64" s="1"/>
       <c r="K64" s="1"/>
     </row>
-    <row r="65" ht="18.0" customHeight="1">
+    <row r="65" spans="1:11" ht="18" customHeight="1">
       <c r="A65" s="1"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -1495,7 +1511,7 @@
       <c r="J65" s="1"/>
       <c r="K65" s="1"/>
     </row>
-    <row r="66" ht="18.0" customHeight="1">
+    <row r="66" spans="1:11" ht="18" customHeight="1">
       <c r="A66" s="1"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -1508,7 +1524,7 @@
       <c r="J66" s="1"/>
       <c r="K66" s="1"/>
     </row>
-    <row r="67" ht="18.0" customHeight="1">
+    <row r="67" spans="1:11" ht="18" customHeight="1">
       <c r="A67" s="1"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -1521,7 +1537,7 @@
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
     </row>
-    <row r="68" ht="18.0" customHeight="1">
+    <row r="68" spans="1:11" ht="18" customHeight="1">
       <c r="A68" s="1"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -1534,7 +1550,7 @@
       <c r="J68" s="1"/>
       <c r="K68" s="1"/>
     </row>
-    <row r="69" ht="18.0" customHeight="1">
+    <row r="69" spans="1:11" ht="18" customHeight="1">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -1547,7 +1563,7 @@
       <c r="J69" s="1"/>
       <c r="K69" s="1"/>
     </row>
-    <row r="70" ht="18.0" customHeight="1">
+    <row r="70" spans="1:11" ht="18" customHeight="1">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -1560,7 +1576,7 @@
       <c r="J70" s="1"/>
       <c r="K70" s="1"/>
     </row>
-    <row r="71" ht="18.0" customHeight="1">
+    <row r="71" spans="1:11" ht="18" customHeight="1">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -1573,7 +1589,7 @@
       <c r="J71" s="1"/>
       <c r="K71" s="1"/>
     </row>
-    <row r="72" ht="18.0" customHeight="1">
+    <row r="72" spans="1:11" ht="18" customHeight="1">
       <c r="A72" s="1"/>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -1586,7 +1602,7 @@
       <c r="J72" s="1"/>
       <c r="K72" s="1"/>
     </row>
-    <row r="73" ht="18.0" customHeight="1">
+    <row r="73" spans="1:11" ht="18" customHeight="1">
       <c r="A73" s="1"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -1599,7 +1615,7 @@
       <c r="J73" s="1"/>
       <c r="K73" s="1"/>
     </row>
-    <row r="74" ht="18.0" customHeight="1">
+    <row r="74" spans="1:11" ht="18" customHeight="1">
       <c r="A74" s="1"/>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -1612,7 +1628,7 @@
       <c r="J74" s="1"/>
       <c r="K74" s="1"/>
     </row>
-    <row r="75" ht="18.0" customHeight="1">
+    <row r="75" spans="1:11" ht="18" customHeight="1">
       <c r="A75" s="1"/>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -1625,7 +1641,7 @@
       <c r="J75" s="1"/>
       <c r="K75" s="1"/>
     </row>
-    <row r="76" ht="18.0" customHeight="1">
+    <row r="76" spans="1:11" ht="18" customHeight="1">
       <c r="A76" s="1"/>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -1638,7 +1654,7 @@
       <c r="J76" s="1"/>
       <c r="K76" s="1"/>
     </row>
-    <row r="77" ht="18.0" customHeight="1">
+    <row r="77" spans="1:11" ht="18" customHeight="1">
       <c r="A77" s="1"/>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -1651,7 +1667,7 @@
       <c r="J77" s="1"/>
       <c r="K77" s="1"/>
     </row>
-    <row r="78" ht="18.0" customHeight="1">
+    <row r="78" spans="1:11" ht="18" customHeight="1">
       <c r="A78" s="1"/>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -1664,7 +1680,7 @@
       <c r="J78" s="1"/>
       <c r="K78" s="1"/>
     </row>
-    <row r="79" ht="18.0" customHeight="1">
+    <row r="79" spans="1:11" ht="18" customHeight="1">
       <c r="A79" s="1"/>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -1677,7 +1693,7 @@
       <c r="J79" s="1"/>
       <c r="K79" s="1"/>
     </row>
-    <row r="80" ht="18.0" customHeight="1">
+    <row r="80" spans="1:11" ht="18" customHeight="1">
       <c r="A80" s="1"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -1690,7 +1706,7 @@
       <c r="J80" s="1"/>
       <c r="K80" s="1"/>
     </row>
-    <row r="81" ht="18.0" customHeight="1">
+    <row r="81" spans="1:11" ht="18" customHeight="1">
       <c r="A81" s="1"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -1703,7 +1719,7 @@
       <c r="J81" s="1"/>
       <c r="K81" s="1"/>
     </row>
-    <row r="82" ht="18.0" customHeight="1">
+    <row r="82" spans="1:11" ht="18" customHeight="1">
       <c r="A82" s="1"/>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -1716,7 +1732,7 @@
       <c r="J82" s="1"/>
       <c r="K82" s="1"/>
     </row>
-    <row r="83" ht="18.0" customHeight="1">
+    <row r="83" spans="1:11" ht="18" customHeight="1">
       <c r="A83" s="1"/>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -1729,7 +1745,7 @@
       <c r="J83" s="1"/>
       <c r="K83" s="1"/>
     </row>
-    <row r="84" ht="18.0" customHeight="1">
+    <row r="84" spans="1:11" ht="18" customHeight="1">
       <c r="A84" s="1"/>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -1742,7 +1758,7 @@
       <c r="J84" s="1"/>
       <c r="K84" s="1"/>
     </row>
-    <row r="85" ht="18.0" customHeight="1">
+    <row r="85" spans="1:11" ht="18" customHeight="1">
       <c r="A85" s="1"/>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -1755,7 +1771,7 @@
       <c r="J85" s="1"/>
       <c r="K85" s="1"/>
     </row>
-    <row r="86" ht="18.0" customHeight="1">
+    <row r="86" spans="1:11" ht="18" customHeight="1">
       <c r="A86" s="1"/>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -1768,7 +1784,7 @@
       <c r="J86" s="1"/>
       <c r="K86" s="1"/>
     </row>
-    <row r="87" ht="18.0" customHeight="1">
+    <row r="87" spans="1:11" ht="18" customHeight="1">
       <c r="A87" s="1"/>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -1781,7 +1797,7 @@
       <c r="J87" s="1"/>
       <c r="K87" s="1"/>
     </row>
-    <row r="88" ht="18.0" customHeight="1">
+    <row r="88" spans="1:11" ht="18" customHeight="1">
       <c r="A88" s="1"/>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -1794,7 +1810,7 @@
       <c r="J88" s="1"/>
       <c r="K88" s="1"/>
     </row>
-    <row r="89" ht="18.0" customHeight="1">
+    <row r="89" spans="1:11" ht="18" customHeight="1">
       <c r="A89" s="1"/>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -1807,7 +1823,7 @@
       <c r="J89" s="1"/>
       <c r="K89" s="1"/>
     </row>
-    <row r="90" ht="18.0" customHeight="1">
+    <row r="90" spans="1:11" ht="18" customHeight="1">
       <c r="A90" s="1"/>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -1820,7 +1836,7 @@
       <c r="J90" s="1"/>
       <c r="K90" s="1"/>
     </row>
-    <row r="91" ht="18.0" customHeight="1">
+    <row r="91" spans="1:11" ht="18" customHeight="1">
       <c r="A91" s="1"/>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -1833,7 +1849,7 @@
       <c r="J91" s="1"/>
       <c r="K91" s="1"/>
     </row>
-    <row r="92" ht="18.0" customHeight="1">
+    <row r="92" spans="1:11" ht="18" customHeight="1">
       <c r="A92" s="1"/>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -1846,7 +1862,7 @@
       <c r="J92" s="1"/>
       <c r="K92" s="1"/>
     </row>
-    <row r="93" ht="18.0" customHeight="1">
+    <row r="93" spans="1:11" ht="18" customHeight="1">
       <c r="A93" s="1"/>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -1859,7 +1875,7 @@
       <c r="J93" s="1"/>
       <c r="K93" s="1"/>
     </row>
-    <row r="94" ht="18.0" customHeight="1">
+    <row r="94" spans="1:11" ht="18" customHeight="1">
       <c r="A94" s="1"/>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -1872,7 +1888,7 @@
       <c r="J94" s="1"/>
       <c r="K94" s="1"/>
     </row>
-    <row r="95" ht="18.0" customHeight="1">
+    <row r="95" spans="1:11" ht="18" customHeight="1">
       <c r="A95" s="1"/>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -1885,7 +1901,7 @@
       <c r="J95" s="1"/>
       <c r="K95" s="1"/>
     </row>
-    <row r="96" ht="18.0" customHeight="1">
+    <row r="96" spans="1:11" ht="18" customHeight="1">
       <c r="A96" s="1"/>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -1898,7 +1914,7 @@
       <c r="J96" s="1"/>
       <c r="K96" s="1"/>
     </row>
-    <row r="97" ht="18.0" customHeight="1">
+    <row r="97" spans="1:11" ht="18" customHeight="1">
       <c r="A97" s="1"/>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -1911,7 +1927,7 @@
       <c r="J97" s="1"/>
       <c r="K97" s="1"/>
     </row>
-    <row r="98" ht="18.0" customHeight="1">
+    <row r="98" spans="1:11" ht="18" customHeight="1">
       <c r="A98" s="1"/>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -1924,7 +1940,7 @@
       <c r="J98" s="1"/>
       <c r="K98" s="1"/>
     </row>
-    <row r="99" ht="18.0" customHeight="1">
+    <row r="99" spans="1:11" ht="18" customHeight="1">
       <c r="A99" s="1"/>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -1937,7 +1953,7 @@
       <c r="J99" s="1"/>
       <c r="K99" s="1"/>
     </row>
-    <row r="100" ht="18.0" customHeight="1">
+    <row r="100" spans="1:11" ht="18" customHeight="1">
       <c r="A100" s="1"/>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -1954,99 +1970,97 @@
   <mergeCells count="1">
     <mergeCell ref="A2:E2"/>
   </mergeCells>
-  <printOptions/>
-  <pageMargins bottom="0.787401575" footer="0.0" header="0.0" left="0.511811024" right="0.511811024" top="0.787401575"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K100"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="27.29"/>
-    <col customWidth="1" min="2" max="2" width="22.29"/>
-    <col customWidth="1" min="3" max="3" width="18.29"/>
-    <col customWidth="1" min="4" max="4" width="15.57"/>
-    <col customWidth="1" min="5" max="5" width="20.29"/>
-    <col customWidth="1" min="6" max="6" width="15.71"/>
-    <col customWidth="1" min="7" max="7" width="13.14"/>
-    <col customWidth="1" min="8" max="8" width="21.57"/>
-    <col customWidth="1" min="9" max="9" width="25.14"/>
-    <col customWidth="1" min="10" max="11" width="9.14"/>
+    <col min="1" max="1" width="27.28515625" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" customWidth="1"/>
+    <col min="3" max="3" width="18.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.5703125" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="13.140625" customWidth="1"/>
+    <col min="8" max="8" width="21.5703125" customWidth="1"/>
+    <col min="9" max="9" width="25.140625" customWidth="1"/>
+    <col min="10" max="11" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18.0" customHeight="1">
-      <c r="A1" s="11" t="s">
+    <row r="1" spans="1:11" ht="18" customHeight="1">
+      <c r="A1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-    </row>
-    <row r="2" ht="18.0" customHeight="1">
-      <c r="A2" s="11"/>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+    </row>
+    <row r="2" spans="1:11" ht="18" customHeight="1">
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-      <c r="G2" s="11"/>
-      <c r="H2" s="11"/>
-      <c r="I2" s="11"/>
-      <c r="J2" s="11"/>
-      <c r="K2" s="11"/>
-    </row>
-    <row r="3" ht="18.0" customHeight="1">
-      <c r="A3" s="11" t="s">
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+    </row>
+    <row r="3" spans="1:11" ht="18" customHeight="1">
+      <c r="A3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="11"/>
+      <c r="C3" s="8"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
-    </row>
-    <row r="4" ht="18.0" customHeight="1">
-      <c r="A4" s="2" t="s">
+      <c r="G3" s="8"/>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="J3" s="8"/>
+      <c r="K3" s="8"/>
+    </row>
+    <row r="4" spans="1:11" ht="18" customHeight="1">
+      <c r="A4" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="4"/>
+      <c r="B4" s="25"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="25"/>
+      <c r="E4" s="26"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
-    </row>
-    <row r="5" ht="18.0" customHeight="1">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11" t="s">
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
+    </row>
+    <row r="5" spans="1:11" ht="18" customHeight="1">
+      <c r="A5" s="8"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="1" t="s">
@@ -2056,206 +2070,206 @@
         <v>14</v>
       </c>
       <c r="F5" s="1"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-    </row>
-    <row r="6" ht="18.0" customHeight="1">
-      <c r="A6" s="11" t="s">
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+    </row>
+    <row r="6" spans="1:11" ht="18" customHeight="1">
+      <c r="A6" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="12">
-        <v>7000.0</v>
-      </c>
-      <c r="D6" s="13">
-        <v>4.0</v>
-      </c>
-      <c r="E6" s="1" t="str">
+      <c r="B6" s="8"/>
+      <c r="C6" s="9">
+        <v>7000</v>
+      </c>
+      <c r="D6" s="10">
+        <v>4</v>
+      </c>
+      <c r="E6" s="1">
         <f>C6*D6</f>
-        <v>  28,000.00 </v>
+        <v>28000</v>
       </c>
       <c r="F6" s="1"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-    </row>
-    <row r="7" ht="18.0" customHeight="1">
-      <c r="A7" s="11" t="s">
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+    </row>
+    <row r="7" spans="1:11" ht="18" customHeight="1">
+      <c r="A7" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="13">
+      <c r="C7" s="8"/>
+      <c r="D7" s="10">
         <v>0.3</v>
       </c>
-      <c r="E7" s="1" t="str">
+      <c r="E7" s="1">
         <f>D7*C6</f>
-        <v>  2,100.00 </v>
+        <v>2100</v>
       </c>
       <c r="F7" s="1"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
-    </row>
-    <row r="8" ht="18.0" customHeight="1">
-      <c r="A8" s="11" t="s">
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+    </row>
+    <row r="8" spans="1:11" ht="18" customHeight="1">
+      <c r="A8" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="13">
-        <v>320.0</v>
-      </c>
-      <c r="E8" s="1" t="str">
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="10">
+        <v>320</v>
+      </c>
+      <c r="E8" s="1">
         <f>D8</f>
-        <v>  320.00 </v>
+        <v>320</v>
       </c>
       <c r="F8" s="1"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
-    </row>
-    <row r="9" ht="18.0" customHeight="1">
-      <c r="A9" s="11" t="s">
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+    </row>
+    <row r="9" spans="1:11" ht="18" customHeight="1">
+      <c r="A9" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="13">
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="10">
         <v>6.6</v>
       </c>
-      <c r="E9" s="14" t="str">
+      <c r="E9" s="11">
         <f>D9*C6</f>
-        <v>  46,200.00 </v>
-      </c>
-      <c r="F9" s="14" t="s">
+        <v>46200</v>
+      </c>
+      <c r="F9" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="G9" s="15"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
-    </row>
-    <row r="10" ht="18.0" customHeight="1">
-      <c r="A10" s="11" t="s">
+      <c r="G9" s="12"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+    </row>
+    <row r="10" spans="1:11" ht="18" customHeight="1">
+      <c r="A10" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="16">
-        <v>0.07</v>
-      </c>
-      <c r="C10" s="11"/>
+      <c r="B10" s="13">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C10" s="8"/>
       <c r="D10" s="1"/>
-      <c r="E10" s="1" t="str">
+      <c r="E10" s="1">
         <f>E9*B10</f>
-        <v>  3,234.00 </v>
+        <v>3234.0000000000005</v>
       </c>
       <c r="F10" s="1"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11"/>
-    </row>
-    <row r="11" ht="18.0" customHeight="1">
-      <c r="A11" s="11" t="s">
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+    </row>
+    <row r="11" spans="1:11" ht="18" customHeight="1">
+      <c r="A11" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B11" s="8">
-        <v>0.0</v>
-      </c>
-      <c r="C11" s="11"/>
+      <c r="B11" s="5">
+        <v>0</v>
+      </c>
+      <c r="C11" s="8"/>
       <c r="D11" s="1"/>
-      <c r="E11" s="1" t="str">
+      <c r="E11" s="1">
         <f>E9*B11</f>
-        <v>  -   </v>
+        <v>0</v>
       </c>
       <c r="F11" s="1"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="11"/>
-    </row>
-    <row r="12" ht="18.0" customHeight="1">
-      <c r="A12" s="11" t="s">
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+    </row>
+    <row r="12" spans="1:11" ht="18" customHeight="1">
+      <c r="A12" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B12" s="11"/>
-      <c r="C12" s="11"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
       <c r="D12" s="1"/>
-      <c r="E12" s="14" t="str">
+      <c r="E12" s="11">
         <f>E9-E6-E7-E8-E10-E11</f>
-        <v>  12,546.00 </v>
-      </c>
-      <c r="F12" s="17" t="str">
+        <v>12546</v>
+      </c>
+      <c r="F12" s="14">
         <f>E12/E9</f>
-        <v>27%</v>
-      </c>
-      <c r="G12" s="15" t="s">
+        <v>0.27155844155844155</v>
+      </c>
+      <c r="G12" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="11"/>
-      <c r="K12" s="11"/>
-    </row>
-    <row r="13" ht="18.0" customHeight="1">
-      <c r="A13" s="11"/>
-      <c r="B13" s="11"/>
-      <c r="C13" s="11"/>
+      <c r="H12" s="12"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+    </row>
+    <row r="13" spans="1:11" ht="18" customHeight="1">
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
-      <c r="J13" s="11"/>
-      <c r="K13" s="11"/>
-    </row>
-    <row r="14" ht="18.0" customHeight="1">
-      <c r="A14" s="11"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+    </row>
+    <row r="14" spans="1:11" ht="18" customHeight="1">
+      <c r="A14" s="8"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="11"/>
-    </row>
-    <row r="15" ht="18.0" customHeight="1">
-      <c r="A15" s="11"/>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+    </row>
+    <row r="15" spans="1:11" ht="18" customHeight="1">
+      <c r="A15" s="8"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="11"/>
-      <c r="I15" s="11"/>
-      <c r="J15" s="11"/>
-      <c r="K15" s="11"/>
-    </row>
-    <row r="16" ht="18.0" customHeight="1">
-      <c r="A16" s="11"/>
-      <c r="B16" s="11" t="s">
+      <c r="G15" s="8"/>
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+    </row>
+    <row r="16" spans="1:11" ht="18" customHeight="1">
+      <c r="A16" s="8"/>
+      <c r="B16" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="C16" s="8" t="s">
         <v>26</v>
       </c>
       <c r="D16" s="1" t="s">
@@ -2267,1203 +2281,1201 @@
       <c r="F16" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G16" s="11" t="s">
+      <c r="G16" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="H16" s="11" t="s">
+      <c r="H16" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="I16" s="11" t="s">
+      <c r="I16" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="J16" s="11"/>
-      <c r="K16" s="11"/>
-    </row>
-    <row r="17" ht="18.0" customHeight="1">
-      <c r="A17" s="11" t="s">
+      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
+    </row>
+    <row r="17" spans="1:11" ht="18" customHeight="1">
+      <c r="A17" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="B17" s="11">
-        <v>7000.0</v>
+      <c r="B17" s="8">
+        <v>7000</v>
       </c>
       <c r="C17" s="1">
-        <v>4.0</v>
-      </c>
-      <c r="D17" s="1" t="str">
+        <v>4</v>
+      </c>
+      <c r="D17" s="1">
         <f>B17*C17</f>
-        <v>  28,000.00 </v>
-      </c>
-      <c r="E17" s="18">
-        <v>1.5433</v>
-      </c>
-      <c r="F17" s="1" t="str">
+        <v>28000</v>
+      </c>
+      <c r="E17" s="15">
+        <v>1.5432999999999999</v>
+      </c>
+      <c r="F17" s="1">
         <f>C17*E17</f>
-        <v>  6.17 </v>
-      </c>
-      <c r="G17" s="11">
+        <v>6.1731999999999996</v>
+      </c>
+      <c r="G17" s="8">
         <v>0.18</v>
       </c>
-      <c r="H17" s="1" t="str">
+      <c r="H17" s="1">
         <f>F17*G17</f>
-        <v>  1.11 </v>
-      </c>
-      <c r="I17" s="1" t="str">
+        <v>1.1111759999999999</v>
+      </c>
+      <c r="I17" s="1">
         <f>C17+H17</f>
-        <v>  5.11 </v>
-      </c>
-      <c r="J17" s="11"/>
-      <c r="K17" s="11"/>
-    </row>
-    <row r="18" ht="18.0" customHeight="1">
-      <c r="A18" s="11"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
+        <v>5.1111760000000004</v>
+      </c>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+    </row>
+    <row r="18" spans="1:11" ht="18" customHeight="1">
+      <c r="A18" s="8"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="11"/>
-      <c r="J18" s="11"/>
-      <c r="K18" s="11"/>
-    </row>
-    <row r="19" ht="18.0" customHeight="1">
-      <c r="A19" s="11"/>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+    </row>
+    <row r="19" spans="1:11" ht="18" customHeight="1">
+      <c r="A19" s="8"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
-      <c r="K19" s="11"/>
-    </row>
-    <row r="20" ht="18.0" customHeight="1">
-      <c r="A20" s="11"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+    </row>
+    <row r="20" spans="1:11" ht="18" customHeight="1">
+      <c r="A20" s="8"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="11"/>
-      <c r="K20" s="11"/>
-    </row>
-    <row r="21" ht="18.0" customHeight="1">
-      <c r="A21" s="11"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="11"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
+    </row>
+    <row r="21" spans="1:11" ht="18" customHeight="1">
+      <c r="A21" s="8"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11"/>
-      <c r="J21" s="11"/>
-      <c r="K21" s="11"/>
-    </row>
-    <row r="22" ht="18.0" customHeight="1">
-      <c r="A22" s="11"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="11"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+    </row>
+    <row r="22" spans="1:11" ht="18" customHeight="1">
+      <c r="A22" s="8"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="11"/>
-      <c r="J22" s="11"/>
-      <c r="K22" s="11"/>
-    </row>
-    <row r="23" ht="18.0" customHeight="1">
-      <c r="A23" s="19"/>
-      <c r="B23" s="19" t="s">
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+    </row>
+    <row r="23" spans="1:11" ht="18" customHeight="1">
+      <c r="A23" s="16"/>
+      <c r="B23" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="C23" s="19" t="s">
+      <c r="C23" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="D23" s="20" t="s">
+      <c r="D23" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="E23" s="20" t="s">
+      <c r="E23" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="F23" s="20" t="s">
+      <c r="F23" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="G23" s="11"/>
-      <c r="H23" s="19" t="s">
+      <c r="G23" s="8"/>
+      <c r="H23" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="I23" s="19" t="s">
+      <c r="I23" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="J23" s="19"/>
-      <c r="K23" s="11"/>
-    </row>
-    <row r="24" ht="18.0" customHeight="1">
-      <c r="A24" s="11"/>
-      <c r="B24" s="11"/>
-      <c r="C24" s="11"/>
+      <c r="J23" s="16"/>
+      <c r="K23" s="8"/>
+    </row>
+    <row r="24" spans="1:11" ht="18" customHeight="1">
+      <c r="A24" s="8"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="11"/>
-      <c r="K24" s="11"/>
-    </row>
-    <row r="25" ht="18.0" customHeight="1">
-      <c r="A25" s="21"/>
-      <c r="B25" s="19">
-        <v>5.11</v>
-      </c>
-      <c r="C25" s="19">
+      <c r="G24" s="8"/>
+      <c r="H24" s="8"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
+      <c r="K24" s="8"/>
+    </row>
+    <row r="25" spans="1:11" ht="18" customHeight="1">
+      <c r="A25" s="18"/>
+      <c r="B25" s="16">
+        <v>5.1100000000000003</v>
+      </c>
+      <c r="C25" s="16">
         <v>0.25</v>
       </c>
-      <c r="D25" s="20" t="str">
+      <c r="D25" s="17">
         <f>B25*C25</f>
-        <v>  1.28 </v>
-      </c>
-      <c r="E25" s="20" t="str">
+        <v>1.2775000000000001</v>
+      </c>
+      <c r="E25" s="17">
         <f>B25+D25</f>
-        <v>  6.39 </v>
-      </c>
-      <c r="F25" s="20">
+        <v>6.3875000000000002</v>
+      </c>
+      <c r="F25" s="17">
         <v>0.92</v>
       </c>
-      <c r="G25" s="22" t="str">
+      <c r="G25" s="19">
         <f>E25/F25</f>
-        <v>6.94</v>
-      </c>
-      <c r="H25" s="11">
+        <v>6.9429347826086953</v>
+      </c>
+      <c r="H25" s="8">
         <v>0.85</v>
       </c>
-      <c r="I25" s="23" t="str">
+      <c r="I25" s="20">
         <f>G25/H25</f>
-        <v>8.17</v>
-      </c>
-      <c r="J25" s="11"/>
-      <c r="K25" s="11"/>
-    </row>
-    <row r="26" ht="18.0" customHeight="1">
-      <c r="A26" s="11"/>
-      <c r="B26" s="11"/>
-      <c r="C26" s="11"/>
+        <v>8.1681585677749364</v>
+      </c>
+      <c r="J25" s="8"/>
+      <c r="K25" s="8"/>
+    </row>
+    <row r="26" spans="1:11" ht="18" customHeight="1">
+      <c r="A26" s="8"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11"/>
-      <c r="I26" s="11"/>
-      <c r="J26" s="11"/>
-      <c r="K26" s="11"/>
-    </row>
-    <row r="27" ht="18.0" customHeight="1">
-      <c r="A27" s="11"/>
-      <c r="B27" s="11"/>
-      <c r="C27" s="11"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="8"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+      <c r="K26" s="8"/>
+    </row>
+    <row r="27" spans="1:11" ht="18" customHeight="1">
+      <c r="A27" s="8"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="8"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11"/>
-      <c r="I27" s="11"/>
-      <c r="J27" s="11"/>
-      <c r="K27" s="11"/>
-    </row>
-    <row r="28" ht="18.0" customHeight="1">
-      <c r="A28" s="11"/>
-      <c r="B28" s="11"/>
-      <c r="C28" s="11"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+      <c r="K27" s="8"/>
+    </row>
+    <row r="28" spans="1:11" ht="18" customHeight="1">
+      <c r="A28" s="8"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
-      <c r="I28" s="11"/>
-      <c r="J28" s="11"/>
-      <c r="K28" s="11"/>
-    </row>
-    <row r="29" ht="18.0" customHeight="1">
-      <c r="A29" s="11"/>
-      <c r="B29" s="11"/>
-      <c r="C29" s="11"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="8"/>
+      <c r="K28" s="8"/>
+    </row>
+    <row r="29" spans="1:11" ht="18" customHeight="1">
+      <c r="A29" s="8"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11"/>
-      <c r="I29" s="11"/>
-      <c r="J29" s="11"/>
-      <c r="K29" s="11"/>
-    </row>
-    <row r="30" ht="18.0" customHeight="1">
-      <c r="A30" s="11"/>
-      <c r="B30" s="11"/>
-      <c r="C30" s="11"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="8"/>
+    </row>
+    <row r="30" spans="1:11" ht="18" customHeight="1">
+      <c r="A30" s="8"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
-      <c r="I30" s="11"/>
-      <c r="J30" s="11"/>
-      <c r="K30" s="11"/>
-    </row>
-    <row r="31" ht="18.0" customHeight="1">
-      <c r="A31" s="24" t="s">
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="8"/>
+      <c r="K30" s="8"/>
+    </row>
+    <row r="31" spans="1:11" ht="18" customHeight="1">
+      <c r="A31" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="B31" s="25"/>
-      <c r="C31" s="11"/>
+      <c r="B31" s="22"/>
+      <c r="C31" s="8"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
-      <c r="G31" s="11"/>
-      <c r="H31" s="11"/>
-      <c r="I31" s="11"/>
-      <c r="J31" s="11"/>
-      <c r="K31" s="11"/>
-    </row>
-    <row r="32" ht="18.0" customHeight="1">
-      <c r="A32" s="24" t="s">
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="8"/>
+      <c r="K31" s="8"/>
+    </row>
+    <row r="32" spans="1:11" ht="18" customHeight="1">
+      <c r="A32" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="B32" s="25">
+      <c r="B32" s="22">
         <v>8.17</v>
       </c>
-      <c r="C32" s="11"/>
+      <c r="C32" s="8"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
-      <c r="G32" s="11"/>
-      <c r="H32" s="11"/>
-      <c r="I32" s="11"/>
-      <c r="J32" s="11"/>
-      <c r="K32" s="11"/>
-    </row>
-    <row r="33" ht="18.0" customHeight="1">
-      <c r="A33" s="24" t="s">
+      <c r="G32" s="8"/>
+      <c r="H32" s="8"/>
+      <c r="I32" s="8"/>
+      <c r="J32" s="8"/>
+      <c r="K32" s="8"/>
+    </row>
+    <row r="33" spans="1:11" ht="18" customHeight="1">
+      <c r="A33" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="B33" s="25">
-        <v>-4.0</v>
-      </c>
-      <c r="C33" s="11"/>
+      <c r="B33" s="22">
+        <v>-4</v>
+      </c>
+      <c r="C33" s="8"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="11"/>
-      <c r="I33" s="11"/>
-      <c r="J33" s="11"/>
-      <c r="K33" s="11"/>
-    </row>
-    <row r="34" ht="18.0" customHeight="1">
-      <c r="A34" s="24" t="s">
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="8"/>
+      <c r="K33" s="8"/>
+    </row>
+    <row r="34" spans="1:11" ht="18" customHeight="1">
+      <c r="A34" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="B34" s="25">
-        <v>-1.11</v>
-      </c>
-      <c r="C34" s="11"/>
+      <c r="B34" s="22">
+        <v>-1.1100000000000001</v>
+      </c>
+      <c r="C34" s="8"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
-      <c r="G34" s="11"/>
-      <c r="H34" s="11"/>
-      <c r="I34" s="11"/>
-      <c r="J34" s="11"/>
-      <c r="K34" s="11"/>
-    </row>
-    <row r="35" ht="18.0" customHeight="1">
-      <c r="A35" s="24" t="s">
+      <c r="G34" s="8"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="8"/>
+      <c r="J34" s="8"/>
+      <c r="K34" s="8"/>
+    </row>
+    <row r="35" spans="1:11" ht="18" customHeight="1">
+      <c r="A35" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="B35" s="25">
-        <v>-0.55</v>
-      </c>
-      <c r="C35" s="11"/>
+      <c r="B35" s="22">
+        <v>-0.55000000000000004</v>
+      </c>
+      <c r="C35" s="8"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
-      <c r="G35" s="11"/>
-      <c r="H35" s="11"/>
-      <c r="I35" s="11"/>
-      <c r="J35" s="11"/>
-      <c r="K35" s="11"/>
-    </row>
-    <row r="36" ht="18.0" customHeight="1">
-      <c r="A36" s="24" t="s">
+      <c r="G35" s="8"/>
+      <c r="H35" s="8"/>
+      <c r="I35" s="8"/>
+      <c r="J35" s="8"/>
+      <c r="K35" s="8"/>
+    </row>
+    <row r="36" spans="1:11" ht="18" customHeight="1">
+      <c r="A36" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="B36" s="25">
+      <c r="B36" s="22">
         <v>-0.69</v>
       </c>
-      <c r="C36" s="11"/>
+      <c r="C36" s="8"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
-      <c r="G36" s="11"/>
-      <c r="H36" s="11"/>
-      <c r="I36" s="11"/>
-      <c r="J36" s="11"/>
-      <c r="K36" s="11"/>
-    </row>
-    <row r="37" ht="18.0" customHeight="1">
-      <c r="A37" s="24"/>
-      <c r="B37" s="25"/>
-      <c r="C37" s="11"/>
+      <c r="G36" s="8"/>
+      <c r="H36" s="8"/>
+      <c r="I36" s="8"/>
+      <c r="J36" s="8"/>
+      <c r="K36" s="8"/>
+    </row>
+    <row r="37" spans="1:11" ht="18" customHeight="1">
+      <c r="A37" s="21"/>
+      <c r="B37" s="22"/>
+      <c r="C37" s="8"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
-      <c r="G37" s="11"/>
-      <c r="H37" s="11"/>
-      <c r="I37" s="11"/>
-      <c r="J37" s="11"/>
-      <c r="K37" s="11"/>
-    </row>
-    <row r="38" ht="18.0" customHeight="1">
-      <c r="A38" s="24"/>
-      <c r="B38" s="25"/>
-      <c r="C38" s="11"/>
+      <c r="G37" s="8"/>
+      <c r="H37" s="8"/>
+      <c r="I37" s="8"/>
+      <c r="J37" s="8"/>
+      <c r="K37" s="8"/>
+    </row>
+    <row r="38" spans="1:11" ht="18" customHeight="1">
+      <c r="A38" s="21"/>
+      <c r="B38" s="22"/>
+      <c r="C38" s="8"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
-      <c r="G38" s="11"/>
-      <c r="H38" s="11"/>
-      <c r="I38" s="11"/>
-      <c r="J38" s="11"/>
-      <c r="K38" s="11"/>
-    </row>
-    <row r="39" ht="18.0" customHeight="1">
-      <c r="A39" s="24"/>
-      <c r="B39" s="25"/>
-      <c r="C39" s="11"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8"/>
+      <c r="I38" s="8"/>
+      <c r="J38" s="8"/>
+      <c r="K38" s="8"/>
+    </row>
+    <row r="39" spans="1:11" ht="18" customHeight="1">
+      <c r="A39" s="21"/>
+      <c r="B39" s="22"/>
+      <c r="C39" s="8"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
-      <c r="G39" s="11"/>
-      <c r="H39" s="11"/>
-      <c r="I39" s="11"/>
-      <c r="J39" s="11"/>
-      <c r="K39" s="11"/>
-    </row>
-    <row r="40" ht="18.0" customHeight="1">
-      <c r="A40" s="24"/>
-      <c r="B40" s="25"/>
-      <c r="C40" s="11"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8"/>
+      <c r="I39" s="8"/>
+      <c r="J39" s="8"/>
+      <c r="K39" s="8"/>
+    </row>
+    <row r="40" spans="1:11" ht="18" customHeight="1">
+      <c r="A40" s="21"/>
+      <c r="B40" s="22"/>
+      <c r="C40" s="8"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
-      <c r="G40" s="11"/>
-      <c r="H40" s="11"/>
-      <c r="I40" s="11"/>
-      <c r="J40" s="11"/>
-      <c r="K40" s="11"/>
-    </row>
-    <row r="41" ht="18.0" customHeight="1">
-      <c r="A41" s="24"/>
-      <c r="B41" s="25"/>
-      <c r="C41" s="11"/>
+      <c r="G40" s="8"/>
+      <c r="H40" s="8"/>
+      <c r="I40" s="8"/>
+      <c r="J40" s="8"/>
+      <c r="K40" s="8"/>
+    </row>
+    <row r="41" spans="1:11" ht="18" customHeight="1">
+      <c r="A41" s="21"/>
+      <c r="B41" s="22"/>
+      <c r="C41" s="8"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
-      <c r="G41" s="11"/>
-      <c r="H41" s="11"/>
-      <c r="I41" s="11"/>
-      <c r="J41" s="11"/>
-      <c r="K41" s="11"/>
-    </row>
-    <row r="42" ht="18.0" customHeight="1">
-      <c r="A42" s="24"/>
-      <c r="B42" s="25"/>
-      <c r="C42" s="11"/>
+      <c r="G41" s="8"/>
+      <c r="H41" s="8"/>
+      <c r="I41" s="8"/>
+      <c r="J41" s="8"/>
+      <c r="K41" s="8"/>
+    </row>
+    <row r="42" spans="1:11" ht="18" customHeight="1">
+      <c r="A42" s="21"/>
+      <c r="B42" s="22"/>
+      <c r="C42" s="8"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
-      <c r="G42" s="11"/>
-      <c r="H42" s="11"/>
-      <c r="I42" s="11"/>
-      <c r="J42" s="11"/>
-      <c r="K42" s="11"/>
-    </row>
-    <row r="43" ht="18.0" customHeight="1">
-      <c r="A43" s="24"/>
-      <c r="B43" s="25"/>
-      <c r="C43" s="11"/>
+      <c r="G42" s="8"/>
+      <c r="H42" s="8"/>
+      <c r="I42" s="8"/>
+      <c r="J42" s="8"/>
+      <c r="K42" s="8"/>
+    </row>
+    <row r="43" spans="1:11" ht="18" customHeight="1">
+      <c r="A43" s="21"/>
+      <c r="B43" s="22"/>
+      <c r="C43" s="8"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
-      <c r="G43" s="11"/>
-      <c r="H43" s="11"/>
-      <c r="I43" s="11"/>
-      <c r="J43" s="11"/>
-      <c r="K43" s="11"/>
-    </row>
-    <row r="44" ht="18.0" customHeight="1">
-      <c r="A44" s="24"/>
-      <c r="B44" s="25" t="str">
+      <c r="G43" s="8"/>
+      <c r="H43" s="8"/>
+      <c r="I43" s="8"/>
+      <c r="J43" s="8"/>
+      <c r="K43" s="8"/>
+    </row>
+    <row r="44" spans="1:11" ht="18" customHeight="1">
+      <c r="A44" s="21"/>
+      <c r="B44" s="22">
         <f>SUM(B32:B43)</f>
-        <v>  1.82 </v>
-      </c>
-      <c r="C44" s="21">
-        <v>7000.0</v>
-      </c>
-      <c r="D44" s="26" t="str">
+        <v>1.8199999999999998</v>
+      </c>
+      <c r="C44" s="18">
+        <v>7000</v>
+      </c>
+      <c r="D44" s="23">
         <f>B44*C44</f>
-        <v>  12,740.00 </v>
+        <v>12739.999999999998</v>
       </c>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
-      <c r="G44" s="11"/>
-      <c r="H44" s="11"/>
-      <c r="I44" s="11"/>
-      <c r="J44" s="11"/>
-      <c r="K44" s="11"/>
-    </row>
-    <row r="45" ht="18.0" customHeight="1">
-      <c r="A45" s="11"/>
+      <c r="G44" s="8"/>
+      <c r="H44" s="8"/>
+      <c r="I44" s="8"/>
+      <c r="J44" s="8"/>
+      <c r="K44" s="8"/>
+    </row>
+    <row r="45" spans="1:11" ht="18" customHeight="1">
+      <c r="A45" s="8"/>
       <c r="B45" s="1"/>
-      <c r="C45" s="11"/>
+      <c r="C45" s="8"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
-      <c r="G45" s="11"/>
-      <c r="H45" s="11"/>
-      <c r="I45" s="11"/>
-      <c r="J45" s="11"/>
-      <c r="K45" s="11"/>
-    </row>
-    <row r="46" ht="18.0" customHeight="1">
-      <c r="A46" s="11"/>
-      <c r="B46" s="11"/>
-      <c r="C46" s="11"/>
+      <c r="G45" s="8"/>
+      <c r="H45" s="8"/>
+      <c r="I45" s="8"/>
+      <c r="J45" s="8"/>
+      <c r="K45" s="8"/>
+    </row>
+    <row r="46" spans="1:11" ht="18" customHeight="1">
+      <c r="A46" s="8"/>
+      <c r="B46" s="8"/>
+      <c r="C46" s="8"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
-      <c r="G46" s="11"/>
-      <c r="H46" s="11"/>
-      <c r="I46" s="11"/>
-      <c r="J46" s="11"/>
-      <c r="K46" s="11"/>
-    </row>
-    <row r="47" ht="18.0" customHeight="1">
-      <c r="A47" s="11"/>
-      <c r="B47" s="11"/>
-      <c r="C47" s="11"/>
+      <c r="G46" s="8"/>
+      <c r="H46" s="8"/>
+      <c r="I46" s="8"/>
+      <c r="J46" s="8"/>
+      <c r="K46" s="8"/>
+    </row>
+    <row r="47" spans="1:11" ht="18" customHeight="1">
+      <c r="A47" s="8"/>
+      <c r="B47" s="8"/>
+      <c r="C47" s="8"/>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
-      <c r="G47" s="11"/>
-      <c r="H47" s="11"/>
-      <c r="I47" s="11"/>
-      <c r="J47" s="11"/>
-      <c r="K47" s="11"/>
-    </row>
-    <row r="48" ht="18.0" customHeight="1">
-      <c r="A48" s="11"/>
-      <c r="B48" s="11"/>
-      <c r="C48" s="11"/>
+      <c r="G47" s="8"/>
+      <c r="H47" s="8"/>
+      <c r="I47" s="8"/>
+      <c r="J47" s="8"/>
+      <c r="K47" s="8"/>
+    </row>
+    <row r="48" spans="1:11" ht="18" customHeight="1">
+      <c r="A48" s="8"/>
+      <c r="B48" s="8"/>
+      <c r="C48" s="8"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
-      <c r="G48" s="11"/>
-      <c r="H48" s="11"/>
-      <c r="I48" s="11"/>
-      <c r="J48" s="11"/>
-      <c r="K48" s="11"/>
-    </row>
-    <row r="49" ht="18.0" customHeight="1">
-      <c r="A49" s="11"/>
-      <c r="B49" s="11"/>
-      <c r="C49" s="11"/>
+      <c r="G48" s="8"/>
+      <c r="H48" s="8"/>
+      <c r="I48" s="8"/>
+      <c r="J48" s="8"/>
+      <c r="K48" s="8"/>
+    </row>
+    <row r="49" spans="1:11" ht="18" customHeight="1">
+      <c r="A49" s="8"/>
+      <c r="B49" s="8"/>
+      <c r="C49" s="8"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
-      <c r="G49" s="11"/>
-      <c r="H49" s="11"/>
-      <c r="I49" s="11"/>
-      <c r="J49" s="11"/>
-      <c r="K49" s="11"/>
-    </row>
-    <row r="50" ht="18.0" customHeight="1">
-      <c r="A50" s="11"/>
-      <c r="B50" s="11"/>
-      <c r="C50" s="11"/>
+      <c r="G49" s="8"/>
+      <c r="H49" s="8"/>
+      <c r="I49" s="8"/>
+      <c r="J49" s="8"/>
+      <c r="K49" s="8"/>
+    </row>
+    <row r="50" spans="1:11" ht="18" customHeight="1">
+      <c r="A50" s="8"/>
+      <c r="B50" s="8"/>
+      <c r="C50" s="8"/>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
-      <c r="G50" s="11"/>
-      <c r="H50" s="11"/>
-      <c r="I50" s="11"/>
-      <c r="J50" s="11"/>
-      <c r="K50" s="11"/>
-    </row>
-    <row r="51" ht="18.0" customHeight="1">
-      <c r="A51" s="11"/>
-      <c r="B51" s="11"/>
-      <c r="C51" s="11"/>
+      <c r="G50" s="8"/>
+      <c r="H50" s="8"/>
+      <c r="I50" s="8"/>
+      <c r="J50" s="8"/>
+      <c r="K50" s="8"/>
+    </row>
+    <row r="51" spans="1:11" ht="18" customHeight="1">
+      <c r="A51" s="8"/>
+      <c r="B51" s="8"/>
+      <c r="C51" s="8"/>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
-      <c r="G51" s="11"/>
-      <c r="H51" s="11"/>
-      <c r="I51" s="11"/>
-      <c r="J51" s="11"/>
-      <c r="K51" s="11"/>
-    </row>
-    <row r="52" ht="18.0" customHeight="1">
-      <c r="A52" s="11"/>
-      <c r="B52" s="11"/>
-      <c r="C52" s="11"/>
+      <c r="G51" s="8"/>
+      <c r="H51" s="8"/>
+      <c r="I51" s="8"/>
+      <c r="J51" s="8"/>
+      <c r="K51" s="8"/>
+    </row>
+    <row r="52" spans="1:11" ht="18" customHeight="1">
+      <c r="A52" s="8"/>
+      <c r="B52" s="8"/>
+      <c r="C52" s="8"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
-      <c r="G52" s="11"/>
-      <c r="H52" s="11"/>
-      <c r="I52" s="11"/>
-      <c r="J52" s="11"/>
-      <c r="K52" s="11"/>
-    </row>
-    <row r="53" ht="18.0" customHeight="1">
-      <c r="A53" s="11"/>
-      <c r="B53" s="11"/>
-      <c r="C53" s="11"/>
+      <c r="G52" s="8"/>
+      <c r="H52" s="8"/>
+      <c r="I52" s="8"/>
+      <c r="J52" s="8"/>
+      <c r="K52" s="8"/>
+    </row>
+    <row r="53" spans="1:11" ht="18" customHeight="1">
+      <c r="A53" s="8"/>
+      <c r="B53" s="8"/>
+      <c r="C53" s="8"/>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
-      <c r="G53" s="11"/>
-      <c r="H53" s="11"/>
-      <c r="I53" s="11"/>
-      <c r="J53" s="11"/>
-      <c r="K53" s="11"/>
-    </row>
-    <row r="54" ht="18.0" customHeight="1">
-      <c r="A54" s="11"/>
-      <c r="B54" s="11"/>
-      <c r="C54" s="11"/>
+      <c r="G53" s="8"/>
+      <c r="H53" s="8"/>
+      <c r="I53" s="8"/>
+      <c r="J53" s="8"/>
+      <c r="K53" s="8"/>
+    </row>
+    <row r="54" spans="1:11" ht="18" customHeight="1">
+      <c r="A54" s="8"/>
+      <c r="B54" s="8"/>
+      <c r="C54" s="8"/>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
-      <c r="G54" s="11"/>
-      <c r="H54" s="11"/>
-      <c r="I54" s="11"/>
-      <c r="J54" s="11"/>
-      <c r="K54" s="11"/>
-    </row>
-    <row r="55" ht="18.0" customHeight="1">
-      <c r="A55" s="11"/>
-      <c r="B55" s="11"/>
-      <c r="C55" s="11"/>
+      <c r="G54" s="8"/>
+      <c r="H54" s="8"/>
+      <c r="I54" s="8"/>
+      <c r="J54" s="8"/>
+      <c r="K54" s="8"/>
+    </row>
+    <row r="55" spans="1:11" ht="18" customHeight="1">
+      <c r="A55" s="8"/>
+      <c r="B55" s="8"/>
+      <c r="C55" s="8"/>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
-      <c r="G55" s="11"/>
-      <c r="H55" s="11"/>
-      <c r="I55" s="11"/>
-      <c r="J55" s="11"/>
-      <c r="K55" s="11"/>
-    </row>
-    <row r="56" ht="18.0" customHeight="1">
-      <c r="A56" s="11"/>
-      <c r="B56" s="11"/>
-      <c r="C56" s="11"/>
+      <c r="G55" s="8"/>
+      <c r="H55" s="8"/>
+      <c r="I55" s="8"/>
+      <c r="J55" s="8"/>
+      <c r="K55" s="8"/>
+    </row>
+    <row r="56" spans="1:11" ht="18" customHeight="1">
+      <c r="A56" s="8"/>
+      <c r="B56" s="8"/>
+      <c r="C56" s="8"/>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
-      <c r="G56" s="11"/>
-      <c r="H56" s="11"/>
-      <c r="I56" s="11"/>
-      <c r="J56" s="11"/>
-      <c r="K56" s="11"/>
-    </row>
-    <row r="57" ht="18.0" customHeight="1">
-      <c r="A57" s="11"/>
-      <c r="B57" s="11"/>
-      <c r="C57" s="11"/>
+      <c r="G56" s="8"/>
+      <c r="H56" s="8"/>
+      <c r="I56" s="8"/>
+      <c r="J56" s="8"/>
+      <c r="K56" s="8"/>
+    </row>
+    <row r="57" spans="1:11" ht="18" customHeight="1">
+      <c r="A57" s="8"/>
+      <c r="B57" s="8"/>
+      <c r="C57" s="8"/>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
-      <c r="G57" s="11"/>
-      <c r="H57" s="11"/>
-      <c r="I57" s="11"/>
-      <c r="J57" s="11"/>
-      <c r="K57" s="11"/>
-    </row>
-    <row r="58" ht="18.0" customHeight="1">
-      <c r="A58" s="11"/>
-      <c r="B58" s="11"/>
-      <c r="C58" s="11"/>
+      <c r="G57" s="8"/>
+      <c r="H57" s="8"/>
+      <c r="I57" s="8"/>
+      <c r="J57" s="8"/>
+      <c r="K57" s="8"/>
+    </row>
+    <row r="58" spans="1:11" ht="18" customHeight="1">
+      <c r="A58" s="8"/>
+      <c r="B58" s="8"/>
+      <c r="C58" s="8"/>
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
-      <c r="G58" s="11"/>
-      <c r="H58" s="11"/>
-      <c r="I58" s="11"/>
-      <c r="J58" s="11"/>
-      <c r="K58" s="11"/>
-    </row>
-    <row r="59" ht="18.0" customHeight="1">
-      <c r="A59" s="11"/>
-      <c r="B59" s="11"/>
-      <c r="C59" s="11"/>
+      <c r="G58" s="8"/>
+      <c r="H58" s="8"/>
+      <c r="I58" s="8"/>
+      <c r="J58" s="8"/>
+      <c r="K58" s="8"/>
+    </row>
+    <row r="59" spans="1:11" ht="18" customHeight="1">
+      <c r="A59" s="8"/>
+      <c r="B59" s="8"/>
+      <c r="C59" s="8"/>
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
-      <c r="G59" s="11"/>
-      <c r="H59" s="11"/>
-      <c r="I59" s="11"/>
-      <c r="J59" s="11"/>
-      <c r="K59" s="11"/>
-    </row>
-    <row r="60" ht="18.0" customHeight="1">
-      <c r="A60" s="11"/>
-      <c r="B60" s="11"/>
-      <c r="C60" s="11"/>
+      <c r="G59" s="8"/>
+      <c r="H59" s="8"/>
+      <c r="I59" s="8"/>
+      <c r="J59" s="8"/>
+      <c r="K59" s="8"/>
+    </row>
+    <row r="60" spans="1:11" ht="18" customHeight="1">
+      <c r="A60" s="8"/>
+      <c r="B60" s="8"/>
+      <c r="C60" s="8"/>
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
-      <c r="G60" s="11"/>
-      <c r="H60" s="11"/>
-      <c r="I60" s="11"/>
-      <c r="J60" s="11"/>
-      <c r="K60" s="11"/>
-    </row>
-    <row r="61" ht="18.0" customHeight="1">
-      <c r="A61" s="11"/>
-      <c r="B61" s="11"/>
-      <c r="C61" s="11"/>
+      <c r="G60" s="8"/>
+      <c r="H60" s="8"/>
+      <c r="I60" s="8"/>
+      <c r="J60" s="8"/>
+      <c r="K60" s="8"/>
+    </row>
+    <row r="61" spans="1:11" ht="18" customHeight="1">
+      <c r="A61" s="8"/>
+      <c r="B61" s="8"/>
+      <c r="C61" s="8"/>
       <c r="D61" s="1"/>
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
-      <c r="G61" s="11"/>
-      <c r="H61" s="11"/>
-      <c r="I61" s="11"/>
-      <c r="J61" s="11"/>
-      <c r="K61" s="11"/>
-    </row>
-    <row r="62" ht="18.0" customHeight="1">
-      <c r="A62" s="11"/>
-      <c r="B62" s="11"/>
-      <c r="C62" s="11"/>
+      <c r="G61" s="8"/>
+      <c r="H61" s="8"/>
+      <c r="I61" s="8"/>
+      <c r="J61" s="8"/>
+      <c r="K61" s="8"/>
+    </row>
+    <row r="62" spans="1:11" ht="18" customHeight="1">
+      <c r="A62" s="8"/>
+      <c r="B62" s="8"/>
+      <c r="C62" s="8"/>
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
-      <c r="G62" s="11"/>
-      <c r="H62" s="11"/>
-      <c r="I62" s="11"/>
-      <c r="J62" s="11"/>
-      <c r="K62" s="11"/>
-    </row>
-    <row r="63" ht="18.0" customHeight="1">
-      <c r="A63" s="11"/>
-      <c r="B63" s="11"/>
-      <c r="C63" s="11"/>
+      <c r="G62" s="8"/>
+      <c r="H62" s="8"/>
+      <c r="I62" s="8"/>
+      <c r="J62" s="8"/>
+      <c r="K62" s="8"/>
+    </row>
+    <row r="63" spans="1:11" ht="18" customHeight="1">
+      <c r="A63" s="8"/>
+      <c r="B63" s="8"/>
+      <c r="C63" s="8"/>
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
-      <c r="G63" s="11"/>
-      <c r="H63" s="11"/>
-      <c r="I63" s="11"/>
-      <c r="J63" s="11"/>
-      <c r="K63" s="11"/>
-    </row>
-    <row r="64" ht="18.0" customHeight="1">
-      <c r="A64" s="11"/>
-      <c r="B64" s="11"/>
-      <c r="C64" s="11"/>
+      <c r="G63" s="8"/>
+      <c r="H63" s="8"/>
+      <c r="I63" s="8"/>
+      <c r="J63" s="8"/>
+      <c r="K63" s="8"/>
+    </row>
+    <row r="64" spans="1:11" ht="18" customHeight="1">
+      <c r="A64" s="8"/>
+      <c r="B64" s="8"/>
+      <c r="C64" s="8"/>
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
       <c r="F64" s="1"/>
-      <c r="G64" s="11"/>
-      <c r="H64" s="11"/>
-      <c r="I64" s="11"/>
-      <c r="J64" s="11"/>
-      <c r="K64" s="11"/>
-    </row>
-    <row r="65" ht="18.0" customHeight="1">
-      <c r="A65" s="11"/>
-      <c r="B65" s="11"/>
-      <c r="C65" s="11"/>
+      <c r="G64" s="8"/>
+      <c r="H64" s="8"/>
+      <c r="I64" s="8"/>
+      <c r="J64" s="8"/>
+      <c r="K64" s="8"/>
+    </row>
+    <row r="65" spans="1:11" ht="18" customHeight="1">
+      <c r="A65" s="8"/>
+      <c r="B65" s="8"/>
+      <c r="C65" s="8"/>
       <c r="D65" s="1"/>
       <c r="E65" s="1"/>
       <c r="F65" s="1"/>
-      <c r="G65" s="11"/>
-      <c r="H65" s="11"/>
-      <c r="I65" s="11"/>
-      <c r="J65" s="11"/>
-      <c r="K65" s="11"/>
-    </row>
-    <row r="66" ht="18.0" customHeight="1">
-      <c r="A66" s="11"/>
-      <c r="B66" s="11"/>
-      <c r="C66" s="11"/>
+      <c r="G65" s="8"/>
+      <c r="H65" s="8"/>
+      <c r="I65" s="8"/>
+      <c r="J65" s="8"/>
+      <c r="K65" s="8"/>
+    </row>
+    <row r="66" spans="1:11" ht="18" customHeight="1">
+      <c r="A66" s="8"/>
+      <c r="B66" s="8"/>
+      <c r="C66" s="8"/>
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
       <c r="F66" s="1"/>
-      <c r="G66" s="11"/>
-      <c r="H66" s="11"/>
-      <c r="I66" s="11"/>
-      <c r="J66" s="11"/>
-      <c r="K66" s="11"/>
-    </row>
-    <row r="67" ht="18.0" customHeight="1">
-      <c r="A67" s="11"/>
-      <c r="B67" s="11"/>
-      <c r="C67" s="11"/>
+      <c r="G66" s="8"/>
+      <c r="H66" s="8"/>
+      <c r="I66" s="8"/>
+      <c r="J66" s="8"/>
+      <c r="K66" s="8"/>
+    </row>
+    <row r="67" spans="1:11" ht="18" customHeight="1">
+      <c r="A67" s="8"/>
+      <c r="B67" s="8"/>
+      <c r="C67" s="8"/>
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
       <c r="F67" s="1"/>
-      <c r="G67" s="11"/>
-      <c r="H67" s="11"/>
-      <c r="I67" s="11"/>
-      <c r="J67" s="11"/>
-      <c r="K67" s="11"/>
-    </row>
-    <row r="68" ht="18.0" customHeight="1">
-      <c r="A68" s="11"/>
-      <c r="B68" s="11"/>
-      <c r="C68" s="11"/>
+      <c r="G67" s="8"/>
+      <c r="H67" s="8"/>
+      <c r="I67" s="8"/>
+      <c r="J67" s="8"/>
+      <c r="K67" s="8"/>
+    </row>
+    <row r="68" spans="1:11" ht="18" customHeight="1">
+      <c r="A68" s="8"/>
+      <c r="B68" s="8"/>
+      <c r="C68" s="8"/>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
-      <c r="G68" s="11"/>
-      <c r="H68" s="11"/>
-      <c r="I68" s="11"/>
-      <c r="J68" s="11"/>
-      <c r="K68" s="11"/>
-    </row>
-    <row r="69" ht="18.0" customHeight="1">
-      <c r="A69" s="11"/>
-      <c r="B69" s="11"/>
-      <c r="C69" s="11"/>
+      <c r="G68" s="8"/>
+      <c r="H68" s="8"/>
+      <c r="I68" s="8"/>
+      <c r="J68" s="8"/>
+      <c r="K68" s="8"/>
+    </row>
+    <row r="69" spans="1:11" ht="18" customHeight="1">
+      <c r="A69" s="8"/>
+      <c r="B69" s="8"/>
+      <c r="C69" s="8"/>
       <c r="D69" s="1"/>
       <c r="E69" s="1"/>
       <c r="F69" s="1"/>
-      <c r="G69" s="11"/>
-      <c r="H69" s="11"/>
-      <c r="I69" s="11"/>
-      <c r="J69" s="11"/>
-      <c r="K69" s="11"/>
-    </row>
-    <row r="70" ht="18.0" customHeight="1">
-      <c r="A70" s="11"/>
-      <c r="B70" s="11"/>
-      <c r="C70" s="11"/>
+      <c r="G69" s="8"/>
+      <c r="H69" s="8"/>
+      <c r="I69" s="8"/>
+      <c r="J69" s="8"/>
+      <c r="K69" s="8"/>
+    </row>
+    <row r="70" spans="1:11" ht="18" customHeight="1">
+      <c r="A70" s="8"/>
+      <c r="B70" s="8"/>
+      <c r="C70" s="8"/>
       <c r="D70" s="1"/>
       <c r="E70" s="1"/>
       <c r="F70" s="1"/>
-      <c r="G70" s="11"/>
-      <c r="H70" s="11"/>
-      <c r="I70" s="11"/>
-      <c r="J70" s="11"/>
-      <c r="K70" s="11"/>
-    </row>
-    <row r="71" ht="18.0" customHeight="1">
-      <c r="A71" s="11"/>
-      <c r="B71" s="11"/>
-      <c r="C71" s="11"/>
+      <c r="G70" s="8"/>
+      <c r="H70" s="8"/>
+      <c r="I70" s="8"/>
+      <c r="J70" s="8"/>
+      <c r="K70" s="8"/>
+    </row>
+    <row r="71" spans="1:11" ht="18" customHeight="1">
+      <c r="A71" s="8"/>
+      <c r="B71" s="8"/>
+      <c r="C71" s="8"/>
       <c r="D71" s="1"/>
       <c r="E71" s="1"/>
       <c r="F71" s="1"/>
-      <c r="G71" s="11"/>
-      <c r="H71" s="11"/>
-      <c r="I71" s="11"/>
-      <c r="J71" s="11"/>
-      <c r="K71" s="11"/>
-    </row>
-    <row r="72" ht="18.0" customHeight="1">
-      <c r="A72" s="11"/>
-      <c r="B72" s="11"/>
-      <c r="C72" s="11"/>
+      <c r="G71" s="8"/>
+      <c r="H71" s="8"/>
+      <c r="I71" s="8"/>
+      <c r="J71" s="8"/>
+      <c r="K71" s="8"/>
+    </row>
+    <row r="72" spans="1:11" ht="18" customHeight="1">
+      <c r="A72" s="8"/>
+      <c r="B72" s="8"/>
+      <c r="C72" s="8"/>
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
       <c r="F72" s="1"/>
-      <c r="G72" s="11"/>
-      <c r="H72" s="11"/>
-      <c r="I72" s="11"/>
-      <c r="J72" s="11"/>
-      <c r="K72" s="11"/>
-    </row>
-    <row r="73" ht="18.0" customHeight="1">
-      <c r="A73" s="11"/>
-      <c r="B73" s="11"/>
-      <c r="C73" s="11"/>
+      <c r="G72" s="8"/>
+      <c r="H72" s="8"/>
+      <c r="I72" s="8"/>
+      <c r="J72" s="8"/>
+      <c r="K72" s="8"/>
+    </row>
+    <row r="73" spans="1:11" ht="18" customHeight="1">
+      <c r="A73" s="8"/>
+      <c r="B73" s="8"/>
+      <c r="C73" s="8"/>
       <c r="D73" s="1"/>
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
-      <c r="G73" s="11"/>
-      <c r="H73" s="11"/>
-      <c r="I73" s="11"/>
-      <c r="J73" s="11"/>
-      <c r="K73" s="11"/>
-    </row>
-    <row r="74" ht="18.0" customHeight="1">
-      <c r="A74" s="11"/>
-      <c r="B74" s="11"/>
-      <c r="C74" s="11"/>
+      <c r="G73" s="8"/>
+      <c r="H73" s="8"/>
+      <c r="I73" s="8"/>
+      <c r="J73" s="8"/>
+      <c r="K73" s="8"/>
+    </row>
+    <row r="74" spans="1:11" ht="18" customHeight="1">
+      <c r="A74" s="8"/>
+      <c r="B74" s="8"/>
+      <c r="C74" s="8"/>
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
-      <c r="G74" s="11"/>
-      <c r="H74" s="11"/>
-      <c r="I74" s="11"/>
-      <c r="J74" s="11"/>
-      <c r="K74" s="11"/>
-    </row>
-    <row r="75" ht="18.0" customHeight="1">
-      <c r="A75" s="11"/>
-      <c r="B75" s="11"/>
-      <c r="C75" s="11"/>
+      <c r="G74" s="8"/>
+      <c r="H74" s="8"/>
+      <c r="I74" s="8"/>
+      <c r="J74" s="8"/>
+      <c r="K74" s="8"/>
+    </row>
+    <row r="75" spans="1:11" ht="18" customHeight="1">
+      <c r="A75" s="8"/>
+      <c r="B75" s="8"/>
+      <c r="C75" s="8"/>
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
       <c r="F75" s="1"/>
-      <c r="G75" s="11"/>
-      <c r="H75" s="11"/>
-      <c r="I75" s="11"/>
-      <c r="J75" s="11"/>
-      <c r="K75" s="11"/>
-    </row>
-    <row r="76" ht="18.0" customHeight="1">
-      <c r="A76" s="11"/>
-      <c r="B76" s="11"/>
-      <c r="C76" s="11"/>
+      <c r="G75" s="8"/>
+      <c r="H75" s="8"/>
+      <c r="I75" s="8"/>
+      <c r="J75" s="8"/>
+      <c r="K75" s="8"/>
+    </row>
+    <row r="76" spans="1:11" ht="18" customHeight="1">
+      <c r="A76" s="8"/>
+      <c r="B76" s="8"/>
+      <c r="C76" s="8"/>
       <c r="D76" s="1"/>
       <c r="E76" s="1"/>
       <c r="F76" s="1"/>
-      <c r="G76" s="11"/>
-      <c r="H76" s="11"/>
-      <c r="I76" s="11"/>
-      <c r="J76" s="11"/>
-      <c r="K76" s="11"/>
-    </row>
-    <row r="77" ht="18.0" customHeight="1">
-      <c r="A77" s="11"/>
-      <c r="B77" s="11"/>
-      <c r="C77" s="11"/>
+      <c r="G76" s="8"/>
+      <c r="H76" s="8"/>
+      <c r="I76" s="8"/>
+      <c r="J76" s="8"/>
+      <c r="K76" s="8"/>
+    </row>
+    <row r="77" spans="1:11" ht="18" customHeight="1">
+      <c r="A77" s="8"/>
+      <c r="B77" s="8"/>
+      <c r="C77" s="8"/>
       <c r="D77" s="1"/>
       <c r="E77" s="1"/>
       <c r="F77" s="1"/>
-      <c r="G77" s="11"/>
-      <c r="H77" s="11"/>
-      <c r="I77" s="11"/>
-      <c r="J77" s="11"/>
-      <c r="K77" s="11"/>
-    </row>
-    <row r="78" ht="18.0" customHeight="1">
-      <c r="A78" s="11"/>
-      <c r="B78" s="11"/>
-      <c r="C78" s="11"/>
+      <c r="G77" s="8"/>
+      <c r="H77" s="8"/>
+      <c r="I77" s="8"/>
+      <c r="J77" s="8"/>
+      <c r="K77" s="8"/>
+    </row>
+    <row r="78" spans="1:11" ht="18" customHeight="1">
+      <c r="A78" s="8"/>
+      <c r="B78" s="8"/>
+      <c r="C78" s="8"/>
       <c r="D78" s="1"/>
       <c r="E78" s="1"/>
       <c r="F78" s="1"/>
-      <c r="G78" s="11"/>
-      <c r="H78" s="11"/>
-      <c r="I78" s="11"/>
-      <c r="J78" s="11"/>
-      <c r="K78" s="11"/>
-    </row>
-    <row r="79" ht="18.0" customHeight="1">
-      <c r="A79" s="11"/>
-      <c r="B79" s="11"/>
-      <c r="C79" s="11"/>
+      <c r="G78" s="8"/>
+      <c r="H78" s="8"/>
+      <c r="I78" s="8"/>
+      <c r="J78" s="8"/>
+      <c r="K78" s="8"/>
+    </row>
+    <row r="79" spans="1:11" ht="18" customHeight="1">
+      <c r="A79" s="8"/>
+      <c r="B79" s="8"/>
+      <c r="C79" s="8"/>
       <c r="D79" s="1"/>
       <c r="E79" s="1"/>
       <c r="F79" s="1"/>
-      <c r="G79" s="11"/>
-      <c r="H79" s="11"/>
-      <c r="I79" s="11"/>
-      <c r="J79" s="11"/>
-      <c r="K79" s="11"/>
-    </row>
-    <row r="80" ht="18.0" customHeight="1">
-      <c r="A80" s="11"/>
-      <c r="B80" s="11"/>
-      <c r="C80" s="11"/>
+      <c r="G79" s="8"/>
+      <c r="H79" s="8"/>
+      <c r="I79" s="8"/>
+      <c r="J79" s="8"/>
+      <c r="K79" s="8"/>
+    </row>
+    <row r="80" spans="1:11" ht="18" customHeight="1">
+      <c r="A80" s="8"/>
+      <c r="B80" s="8"/>
+      <c r="C80" s="8"/>
       <c r="D80" s="1"/>
       <c r="E80" s="1"/>
       <c r="F80" s="1"/>
-      <c r="G80" s="11"/>
-      <c r="H80" s="11"/>
-      <c r="I80" s="11"/>
-      <c r="J80" s="11"/>
-      <c r="K80" s="11"/>
-    </row>
-    <row r="81" ht="18.0" customHeight="1">
-      <c r="A81" s="11"/>
-      <c r="B81" s="11"/>
-      <c r="C81" s="11"/>
+      <c r="G80" s="8"/>
+      <c r="H80" s="8"/>
+      <c r="I80" s="8"/>
+      <c r="J80" s="8"/>
+      <c r="K80" s="8"/>
+    </row>
+    <row r="81" spans="1:11" ht="18" customHeight="1">
+      <c r="A81" s="8"/>
+      <c r="B81" s="8"/>
+      <c r="C81" s="8"/>
       <c r="D81" s="1"/>
       <c r="E81" s="1"/>
       <c r="F81" s="1"/>
-      <c r="G81" s="11"/>
-      <c r="H81" s="11"/>
-      <c r="I81" s="11"/>
-      <c r="J81" s="11"/>
-      <c r="K81" s="11"/>
-    </row>
-    <row r="82" ht="18.0" customHeight="1">
-      <c r="A82" s="11"/>
-      <c r="B82" s="11"/>
-      <c r="C82" s="11"/>
+      <c r="G81" s="8"/>
+      <c r="H81" s="8"/>
+      <c r="I81" s="8"/>
+      <c r="J81" s="8"/>
+      <c r="K81" s="8"/>
+    </row>
+    <row r="82" spans="1:11" ht="18" customHeight="1">
+      <c r="A82" s="8"/>
+      <c r="B82" s="8"/>
+      <c r="C82" s="8"/>
       <c r="D82" s="1"/>
       <c r="E82" s="1"/>
       <c r="F82" s="1"/>
-      <c r="G82" s="11"/>
-      <c r="H82" s="11"/>
-      <c r="I82" s="11"/>
-      <c r="J82" s="11"/>
-      <c r="K82" s="11"/>
-    </row>
-    <row r="83" ht="18.0" customHeight="1">
-      <c r="A83" s="11"/>
-      <c r="B83" s="11"/>
-      <c r="C83" s="11"/>
+      <c r="G82" s="8"/>
+      <c r="H82" s="8"/>
+      <c r="I82" s="8"/>
+      <c r="J82" s="8"/>
+      <c r="K82" s="8"/>
+    </row>
+    <row r="83" spans="1:11" ht="18" customHeight="1">
+      <c r="A83" s="8"/>
+      <c r="B83" s="8"/>
+      <c r="C83" s="8"/>
       <c r="D83" s="1"/>
       <c r="E83" s="1"/>
       <c r="F83" s="1"/>
-      <c r="G83" s="11"/>
-      <c r="H83" s="11"/>
-      <c r="I83" s="11"/>
-      <c r="J83" s="11"/>
-      <c r="K83" s="11"/>
-    </row>
-    <row r="84" ht="18.0" customHeight="1">
-      <c r="A84" s="11"/>
-      <c r="B84" s="11"/>
-      <c r="C84" s="11"/>
+      <c r="G83" s="8"/>
+      <c r="H83" s="8"/>
+      <c r="I83" s="8"/>
+      <c r="J83" s="8"/>
+      <c r="K83" s="8"/>
+    </row>
+    <row r="84" spans="1:11" ht="18" customHeight="1">
+      <c r="A84" s="8"/>
+      <c r="B84" s="8"/>
+      <c r="C84" s="8"/>
       <c r="D84" s="1"/>
       <c r="E84" s="1"/>
       <c r="F84" s="1"/>
-      <c r="G84" s="11"/>
-      <c r="H84" s="11"/>
-      <c r="I84" s="11"/>
-      <c r="J84" s="11"/>
-      <c r="K84" s="11"/>
-    </row>
-    <row r="85" ht="18.0" customHeight="1">
-      <c r="A85" s="11"/>
-      <c r="B85" s="11"/>
-      <c r="C85" s="11"/>
+      <c r="G84" s="8"/>
+      <c r="H84" s="8"/>
+      <c r="I84" s="8"/>
+      <c r="J84" s="8"/>
+      <c r="K84" s="8"/>
+    </row>
+    <row r="85" spans="1:11" ht="18" customHeight="1">
+      <c r="A85" s="8"/>
+      <c r="B85" s="8"/>
+      <c r="C85" s="8"/>
       <c r="D85" s="1"/>
       <c r="E85" s="1"/>
       <c r="F85" s="1"/>
-      <c r="G85" s="11"/>
-      <c r="H85" s="11"/>
-      <c r="I85" s="11"/>
-      <c r="J85" s="11"/>
-      <c r="K85" s="11"/>
-    </row>
-    <row r="86" ht="18.0" customHeight="1">
-      <c r="A86" s="11"/>
-      <c r="B86" s="11"/>
-      <c r="C86" s="11"/>
+      <c r="G85" s="8"/>
+      <c r="H85" s="8"/>
+      <c r="I85" s="8"/>
+      <c r="J85" s="8"/>
+      <c r="K85" s="8"/>
+    </row>
+    <row r="86" spans="1:11" ht="18" customHeight="1">
+      <c r="A86" s="8"/>
+      <c r="B86" s="8"/>
+      <c r="C86" s="8"/>
       <c r="D86" s="1"/>
       <c r="E86" s="1"/>
       <c r="F86" s="1"/>
-      <c r="G86" s="11"/>
-      <c r="H86" s="11"/>
-      <c r="I86" s="11"/>
-      <c r="J86" s="11"/>
-      <c r="K86" s="11"/>
-    </row>
-    <row r="87" ht="18.0" customHeight="1">
-      <c r="A87" s="11"/>
-      <c r="B87" s="11"/>
-      <c r="C87" s="11"/>
+      <c r="G86" s="8"/>
+      <c r="H86" s="8"/>
+      <c r="I86" s="8"/>
+      <c r="J86" s="8"/>
+      <c r="K86" s="8"/>
+    </row>
+    <row r="87" spans="1:11" ht="18" customHeight="1">
+      <c r="A87" s="8"/>
+      <c r="B87" s="8"/>
+      <c r="C87" s="8"/>
       <c r="D87" s="1"/>
       <c r="E87" s="1"/>
       <c r="F87" s="1"/>
-      <c r="G87" s="11"/>
-      <c r="H87" s="11"/>
-      <c r="I87" s="11"/>
-      <c r="J87" s="11"/>
-      <c r="K87" s="11"/>
-    </row>
-    <row r="88" ht="18.0" customHeight="1">
-      <c r="A88" s="11"/>
-      <c r="B88" s="11"/>
-      <c r="C88" s="11"/>
+      <c r="G87" s="8"/>
+      <c r="H87" s="8"/>
+      <c r="I87" s="8"/>
+      <c r="J87" s="8"/>
+      <c r="K87" s="8"/>
+    </row>
+    <row r="88" spans="1:11" ht="18" customHeight="1">
+      <c r="A88" s="8"/>
+      <c r="B88" s="8"/>
+      <c r="C88" s="8"/>
       <c r="D88" s="1"/>
       <c r="E88" s="1"/>
       <c r="F88" s="1"/>
-      <c r="G88" s="11"/>
-      <c r="H88" s="11"/>
-      <c r="I88" s="11"/>
-      <c r="J88" s="11"/>
-      <c r="K88" s="11"/>
-    </row>
-    <row r="89" ht="18.0" customHeight="1">
-      <c r="A89" s="11"/>
-      <c r="B89" s="11"/>
-      <c r="C89" s="11"/>
+      <c r="G88" s="8"/>
+      <c r="H88" s="8"/>
+      <c r="I88" s="8"/>
+      <c r="J88" s="8"/>
+      <c r="K88" s="8"/>
+    </row>
+    <row r="89" spans="1:11" ht="18" customHeight="1">
+      <c r="A89" s="8"/>
+      <c r="B89" s="8"/>
+      <c r="C89" s="8"/>
       <c r="D89" s="1"/>
       <c r="E89" s="1"/>
       <c r="F89" s="1"/>
-      <c r="G89" s="11"/>
-      <c r="H89" s="11"/>
-      <c r="I89" s="11"/>
-      <c r="J89" s="11"/>
-      <c r="K89" s="11"/>
-    </row>
-    <row r="90" ht="18.0" customHeight="1">
-      <c r="A90" s="11"/>
-      <c r="B90" s="11"/>
-      <c r="C90" s="11"/>
+      <c r="G89" s="8"/>
+      <c r="H89" s="8"/>
+      <c r="I89" s="8"/>
+      <c r="J89" s="8"/>
+      <c r="K89" s="8"/>
+    </row>
+    <row r="90" spans="1:11" ht="18" customHeight="1">
+      <c r="A90" s="8"/>
+      <c r="B90" s="8"/>
+      <c r="C90" s="8"/>
       <c r="D90" s="1"/>
       <c r="E90" s="1"/>
       <c r="F90" s="1"/>
-      <c r="G90" s="11"/>
-      <c r="H90" s="11"/>
-      <c r="I90" s="11"/>
-      <c r="J90" s="11"/>
-      <c r="K90" s="11"/>
-    </row>
-    <row r="91" ht="18.0" customHeight="1">
-      <c r="A91" s="11"/>
-      <c r="B91" s="11"/>
-      <c r="C91" s="11"/>
+      <c r="G90" s="8"/>
+      <c r="H90" s="8"/>
+      <c r="I90" s="8"/>
+      <c r="J90" s="8"/>
+      <c r="K90" s="8"/>
+    </row>
+    <row r="91" spans="1:11" ht="18" customHeight="1">
+      <c r="A91" s="8"/>
+      <c r="B91" s="8"/>
+      <c r="C91" s="8"/>
       <c r="D91" s="1"/>
       <c r="E91" s="1"/>
       <c r="F91" s="1"/>
-      <c r="G91" s="11"/>
-      <c r="H91" s="11"/>
-      <c r="I91" s="11"/>
-      <c r="J91" s="11"/>
-      <c r="K91" s="11"/>
-    </row>
-    <row r="92" ht="18.0" customHeight="1">
-      <c r="A92" s="11"/>
-      <c r="B92" s="11"/>
-      <c r="C92" s="11"/>
+      <c r="G91" s="8"/>
+      <c r="H91" s="8"/>
+      <c r="I91" s="8"/>
+      <c r="J91" s="8"/>
+      <c r="K91" s="8"/>
+    </row>
+    <row r="92" spans="1:11" ht="18" customHeight="1">
+      <c r="A92" s="8"/>
+      <c r="B92" s="8"/>
+      <c r="C92" s="8"/>
       <c r="D92" s="1"/>
       <c r="E92" s="1"/>
       <c r="F92" s="1"/>
-      <c r="G92" s="11"/>
-      <c r="H92" s="11"/>
-      <c r="I92" s="11"/>
-      <c r="J92" s="11"/>
-      <c r="K92" s="11"/>
-    </row>
-    <row r="93" ht="18.0" customHeight="1">
-      <c r="A93" s="11"/>
-      <c r="B93" s="11"/>
-      <c r="C93" s="11"/>
+      <c r="G92" s="8"/>
+      <c r="H92" s="8"/>
+      <c r="I92" s="8"/>
+      <c r="J92" s="8"/>
+      <c r="K92" s="8"/>
+    </row>
+    <row r="93" spans="1:11" ht="18" customHeight="1">
+      <c r="A93" s="8"/>
+      <c r="B93" s="8"/>
+      <c r="C93" s="8"/>
       <c r="D93" s="1"/>
       <c r="E93" s="1"/>
       <c r="F93" s="1"/>
-      <c r="G93" s="11"/>
-      <c r="H93" s="11"/>
-      <c r="I93" s="11"/>
-      <c r="J93" s="11"/>
-      <c r="K93" s="11"/>
-    </row>
-    <row r="94" ht="18.0" customHeight="1">
-      <c r="A94" s="11"/>
-      <c r="B94" s="11"/>
-      <c r="C94" s="11"/>
+      <c r="G93" s="8"/>
+      <c r="H93" s="8"/>
+      <c r="I93" s="8"/>
+      <c r="J93" s="8"/>
+      <c r="K93" s="8"/>
+    </row>
+    <row r="94" spans="1:11" ht="18" customHeight="1">
+      <c r="A94" s="8"/>
+      <c r="B94" s="8"/>
+      <c r="C94" s="8"/>
       <c r="D94" s="1"/>
       <c r="E94" s="1"/>
       <c r="F94" s="1"/>
-      <c r="G94" s="11"/>
-      <c r="H94" s="11"/>
-      <c r="I94" s="11"/>
-      <c r="J94" s="11"/>
-      <c r="K94" s="11"/>
-    </row>
-    <row r="95" ht="18.0" customHeight="1">
-      <c r="A95" s="11"/>
-      <c r="B95" s="11"/>
-      <c r="C95" s="11"/>
+      <c r="G94" s="8"/>
+      <c r="H94" s="8"/>
+      <c r="I94" s="8"/>
+      <c r="J94" s="8"/>
+      <c r="K94" s="8"/>
+    </row>
+    <row r="95" spans="1:11" ht="18" customHeight="1">
+      <c r="A95" s="8"/>
+      <c r="B95" s="8"/>
+      <c r="C95" s="8"/>
       <c r="D95" s="1"/>
       <c r="E95" s="1"/>
       <c r="F95" s="1"/>
-      <c r="G95" s="11"/>
-      <c r="H95" s="11"/>
-      <c r="I95" s="11"/>
-      <c r="J95" s="11"/>
-      <c r="K95" s="11"/>
-    </row>
-    <row r="96" ht="18.0" customHeight="1">
-      <c r="A96" s="11"/>
-      <c r="B96" s="11"/>
-      <c r="C96" s="11"/>
+      <c r="G95" s="8"/>
+      <c r="H95" s="8"/>
+      <c r="I95" s="8"/>
+      <c r="J95" s="8"/>
+      <c r="K95" s="8"/>
+    </row>
+    <row r="96" spans="1:11" ht="18" customHeight="1">
+      <c r="A96" s="8"/>
+      <c r="B96" s="8"/>
+      <c r="C96" s="8"/>
       <c r="D96" s="1"/>
       <c r="E96" s="1"/>
       <c r="F96" s="1"/>
-      <c r="G96" s="11"/>
-      <c r="H96" s="11"/>
-      <c r="I96" s="11"/>
-      <c r="J96" s="11"/>
-      <c r="K96" s="11"/>
-    </row>
-    <row r="97" ht="18.0" customHeight="1">
-      <c r="A97" s="11"/>
-      <c r="B97" s="11"/>
-      <c r="C97" s="11"/>
+      <c r="G96" s="8"/>
+      <c r="H96" s="8"/>
+      <c r="I96" s="8"/>
+      <c r="J96" s="8"/>
+      <c r="K96" s="8"/>
+    </row>
+    <row r="97" spans="1:11" ht="18" customHeight="1">
+      <c r="A97" s="8"/>
+      <c r="B97" s="8"/>
+      <c r="C97" s="8"/>
       <c r="D97" s="1"/>
       <c r="E97" s="1"/>
       <c r="F97" s="1"/>
-      <c r="G97" s="11"/>
-      <c r="H97" s="11"/>
-      <c r="I97" s="11"/>
-      <c r="J97" s="11"/>
-      <c r="K97" s="11"/>
-    </row>
-    <row r="98" ht="18.0" customHeight="1">
-      <c r="A98" s="11"/>
-      <c r="B98" s="11"/>
-      <c r="C98" s="11"/>
+      <c r="G97" s="8"/>
+      <c r="H97" s="8"/>
+      <c r="I97" s="8"/>
+      <c r="J97" s="8"/>
+      <c r="K97" s="8"/>
+    </row>
+    <row r="98" spans="1:11" ht="18" customHeight="1">
+      <c r="A98" s="8"/>
+      <c r="B98" s="8"/>
+      <c r="C98" s="8"/>
       <c r="D98" s="1"/>
       <c r="E98" s="1"/>
       <c r="F98" s="1"/>
-      <c r="G98" s="11"/>
-      <c r="H98" s="11"/>
-      <c r="I98" s="11"/>
-      <c r="J98" s="11"/>
-      <c r="K98" s="11"/>
-    </row>
-    <row r="99" ht="18.0" customHeight="1">
-      <c r="A99" s="11"/>
-      <c r="B99" s="11"/>
-      <c r="C99" s="11"/>
+      <c r="G98" s="8"/>
+      <c r="H98" s="8"/>
+      <c r="I98" s="8"/>
+      <c r="J98" s="8"/>
+      <c r="K98" s="8"/>
+    </row>
+    <row r="99" spans="1:11" ht="18" customHeight="1">
+      <c r="A99" s="8"/>
+      <c r="B99" s="8"/>
+      <c r="C99" s="8"/>
       <c r="D99" s="1"/>
       <c r="E99" s="1"/>
       <c r="F99" s="1"/>
-      <c r="G99" s="11"/>
-      <c r="H99" s="11"/>
-      <c r="I99" s="11"/>
-      <c r="J99" s="11"/>
-      <c r="K99" s="11"/>
-    </row>
-    <row r="100" ht="18.0" customHeight="1">
-      <c r="A100" s="11"/>
-      <c r="B100" s="11"/>
-      <c r="C100" s="11"/>
+      <c r="G99" s="8"/>
+      <c r="H99" s="8"/>
+      <c r="I99" s="8"/>
+      <c r="J99" s="8"/>
+      <c r="K99" s="8"/>
+    </row>
+    <row r="100" spans="1:11" ht="18" customHeight="1">
+      <c r="A100" s="8"/>
+      <c r="B100" s="8"/>
+      <c r="C100" s="8"/>
       <c r="D100" s="1"/>
       <c r="E100" s="1"/>
       <c r="F100" s="1"/>
-      <c r="G100" s="11"/>
-      <c r="H100" s="11"/>
-      <c r="I100" s="11"/>
-      <c r="J100" s="11"/>
-      <c r="K100" s="11"/>
+      <c r="G100" s="8"/>
+      <c r="H100" s="8"/>
+      <c r="I100" s="8"/>
+      <c r="J100" s="8"/>
+      <c r="K100" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A4:E4"/>
   </mergeCells>
-  <printOptions/>
-  <pageMargins bottom="0.787401575" footer="0.0" header="0.0" left="0.511811024" right="0.511811024" top="0.787401575"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>